<commit_message>
working on external annotations
</commit_message>
<xml_diff>
--- a/sbmlutils/dfba/diauxic_growth/annotations.xlsx
+++ b/sbmlutils/dfba/diauxic_growth/annotations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="67">
   <si>
     <t xml:space="preserve">pattern</t>
   </si>
@@ -34,10 +34,7 @@
     <t xml:space="preserve">qualifier</t>
   </si>
   <si>
-    <t xml:space="preserve">collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entity</t>
+    <t xml:space="preserve">resource</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -52,16 +49,13 @@
     <t xml:space="preserve">model</t>
   </si>
   <si>
-    <t xml:space="preserve">RDF</t>
+    <t xml:space="preserve">rdf</t>
   </si>
   <si>
     <t xml:space="preserve">BQB_IS_VERSION_OF</t>
   </si>
   <si>
-    <t xml:space="preserve">go</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0006007</t>
+    <t xml:space="preserve">go/GO:0006007</t>
   </si>
   <si>
     <t xml:space="preserve">glucose catabolic process</t>
@@ -79,10 +73,7 @@
     <t xml:space="preserve">BQB_IS</t>
   </si>
   <si>
-    <t xml:space="preserve">uo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UO:0000032</t>
+    <t xml:space="preserve">uo/UO:0000032</t>
   </si>
   <si>
     <t xml:space="preserve">hour</t>
@@ -91,7 +82,7 @@
     <t xml:space="preserve">^m$</t>
   </si>
   <si>
-    <t xml:space="preserve">UO:0000008</t>
+    <t xml:space="preserve">uo/UO:0000008</t>
   </si>
   <si>
     <t xml:space="preserve">meter</t>
@@ -100,7 +91,7 @@
     <t xml:space="preserve">^m2$</t>
   </si>
   <si>
-    <t xml:space="preserve">UO:0000080</t>
+    <t xml:space="preserve">uo/UO:0000080</t>
   </si>
   <si>
     <t xml:space="preserve">square meter</t>
@@ -115,22 +106,16 @@
     <t xml:space="preserve">compartment</t>
   </si>
   <si>
-    <t xml:space="preserve">sbo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBO:0000290</t>
+    <t xml:space="preserve">sbo/SBO:0000290</t>
   </si>
   <si>
     <t xml:space="preserve">physical compartment</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005623</t>
+    <t xml:space="preserve">go/GO:0005623</t>
   </si>
   <si>
-    <t xml:space="preserve">fma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FMA:68646</t>
+    <t xml:space="preserve">fma/FMA:68646</t>
   </si>
   <si>
     <t xml:space="preserve"># species</t>
@@ -142,37 +127,31 @@
     <t xml:space="preserve">species</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000247</t>
+    <t xml:space="preserve">sbo/SBO:0000247</t>
   </si>
   <si>
     <t xml:space="preserve">simple chemical</t>
   </si>
   <si>
-    <t xml:space="preserve">chebi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHEBI:4167</t>
+    <t xml:space="preserve">chebi/CHEBI:4167</t>
   </si>
   <si>
     <t xml:space="preserve">D-glucopyranose</t>
   </si>
   <si>
-    <t xml:space="preserve">kegg.compound</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C00031</t>
+    <t xml:space="preserve">kegg.compound/C00031</t>
   </si>
   <si>
     <t xml:space="preserve">D-Glucose</t>
   </si>
   <si>
-    <t xml:space="preserve">Formula</t>
+    <t xml:space="preserve">formula</t>
   </si>
   <si>
     <t xml:space="preserve">C6H12O6</t>
   </si>
   <si>
-    <t xml:space="preserve">Charge</t>
+    <t xml:space="preserve">charge</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
@@ -181,13 +160,13 @@
     <t xml:space="preserve">Ac</t>
   </si>
   <si>
-    <t xml:space="preserve">CHEBI:15366</t>
+    <t xml:space="preserve">chebi/CHEBI:15366</t>
   </si>
   <si>
     <t xml:space="preserve">acetic acid</t>
   </si>
   <si>
-    <t xml:space="preserve">C00033</t>
+    <t xml:space="preserve">kegg.compound/C00033</t>
   </si>
   <si>
     <t xml:space="preserve">Acetate</t>
@@ -199,13 +178,13 @@
     <t xml:space="preserve">O2</t>
   </si>
   <si>
-    <t xml:space="preserve">CHEBI:15379</t>
+    <t xml:space="preserve">chebi/CHEBI:15379</t>
   </si>
   <si>
     <t xml:space="preserve">dioxygen</t>
   </si>
   <si>
-    <t xml:space="preserve">C00007</t>
+    <t xml:space="preserve">kegg.compound/C00007</t>
   </si>
   <si>
     <t xml:space="preserve">Oxygen</t>
@@ -214,10 +193,7 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">omit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OMIT:0018723</t>
+    <t xml:space="preserve">omit/MI:0018723</t>
   </si>
   <si>
     <t xml:space="preserve"># parameters</t>
@@ -232,13 +208,13 @@
     <t xml:space="preserve">reaction</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000176</t>
+    <t xml:space="preserve">sbo/SBO:0000176</t>
   </si>
   <si>
     <t xml:space="preserve">biochemical reaction</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000629</t>
+    <t xml:space="preserve">sbo/SBO:0000629</t>
   </si>
   <si>
     <t xml:space="preserve">biomass production</t>
@@ -473,23 +449,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:50"/>
+  <dimension ref="A1:AMI50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.2959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.1428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="37.9948979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="55.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="13.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="13.3571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,15 +481,13 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="H1" s="0"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
       <c r="K1" s="0"/>
@@ -1529,18 +1503,17 @@
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="5"/>
+      <c r="H2" s="0"/>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
@@ -2556,30 +2529,27 @@
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
       <c r="K3" s="0"/>
@@ -3595,16 +3565,15 @@
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="H4" s="0"/>
       <c r="I4" s="0"/>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
@@ -4620,16 +4589,1039 @@
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
+      <c r="AG5" s="0"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
+      <c r="AJ5" s="0"/>
+      <c r="AK5" s="0"/>
+      <c r="AL5" s="0"/>
+      <c r="AM5" s="0"/>
+      <c r="AN5" s="0"/>
+      <c r="AO5" s="0"/>
+      <c r="AP5" s="0"/>
+      <c r="AQ5" s="0"/>
+      <c r="AR5" s="0"/>
+      <c r="AS5" s="0"/>
+      <c r="AT5" s="0"/>
+      <c r="AU5" s="0"/>
+      <c r="AV5" s="0"/>
+      <c r="AW5" s="0"/>
+      <c r="AX5" s="0"/>
+      <c r="AY5" s="0"/>
+      <c r="AZ5" s="0"/>
+      <c r="BA5" s="0"/>
+      <c r="BB5" s="0"/>
+      <c r="BC5" s="0"/>
+      <c r="BD5" s="0"/>
+      <c r="BE5" s="0"/>
+      <c r="BF5" s="0"/>
+      <c r="BG5" s="0"/>
+      <c r="BH5" s="0"/>
+      <c r="BI5" s="0"/>
+      <c r="BJ5" s="0"/>
+      <c r="BK5" s="0"/>
+      <c r="BL5" s="0"/>
+      <c r="BM5" s="0"/>
+      <c r="BN5" s="0"/>
+      <c r="BO5" s="0"/>
+      <c r="BP5" s="0"/>
+      <c r="BQ5" s="0"/>
+      <c r="BR5" s="0"/>
+      <c r="BS5" s="0"/>
+      <c r="BT5" s="0"/>
+      <c r="BU5" s="0"/>
+      <c r="BV5" s="0"/>
+      <c r="BW5" s="0"/>
+      <c r="BX5" s="0"/>
+      <c r="BY5" s="0"/>
+      <c r="BZ5" s="0"/>
+      <c r="CA5" s="0"/>
+      <c r="CB5" s="0"/>
+      <c r="CC5" s="0"/>
+      <c r="CD5" s="0"/>
+      <c r="CE5" s="0"/>
+      <c r="CF5" s="0"/>
+      <c r="CG5" s="0"/>
+      <c r="CH5" s="0"/>
+      <c r="CI5" s="0"/>
+      <c r="CJ5" s="0"/>
+      <c r="CK5" s="0"/>
+      <c r="CL5" s="0"/>
+      <c r="CM5" s="0"/>
+      <c r="CN5" s="0"/>
+      <c r="CO5" s="0"/>
+      <c r="CP5" s="0"/>
+      <c r="CQ5" s="0"/>
+      <c r="CR5" s="0"/>
+      <c r="CS5" s="0"/>
+      <c r="CT5" s="0"/>
+      <c r="CU5" s="0"/>
+      <c r="CV5" s="0"/>
+      <c r="CW5" s="0"/>
+      <c r="CX5" s="0"/>
+      <c r="CY5" s="0"/>
+      <c r="CZ5" s="0"/>
+      <c r="DA5" s="0"/>
+      <c r="DB5" s="0"/>
+      <c r="DC5" s="0"/>
+      <c r="DD5" s="0"/>
+      <c r="DE5" s="0"/>
+      <c r="DF5" s="0"/>
+      <c r="DG5" s="0"/>
+      <c r="DH5" s="0"/>
+      <c r="DI5" s="0"/>
+      <c r="DJ5" s="0"/>
+      <c r="DK5" s="0"/>
+      <c r="DL5" s="0"/>
+      <c r="DM5" s="0"/>
+      <c r="DN5" s="0"/>
+      <c r="DO5" s="0"/>
+      <c r="DP5" s="0"/>
+      <c r="DQ5" s="0"/>
+      <c r="DR5" s="0"/>
+      <c r="DS5" s="0"/>
+      <c r="DT5" s="0"/>
+      <c r="DU5" s="0"/>
+      <c r="DV5" s="0"/>
+      <c r="DW5" s="0"/>
+      <c r="DX5" s="0"/>
+      <c r="DY5" s="0"/>
+      <c r="DZ5" s="0"/>
+      <c r="EA5" s="0"/>
+      <c r="EB5" s="0"/>
+      <c r="EC5" s="0"/>
+      <c r="ED5" s="0"/>
+      <c r="EE5" s="0"/>
+      <c r="EF5" s="0"/>
+      <c r="EG5" s="0"/>
+      <c r="EH5" s="0"/>
+      <c r="EI5" s="0"/>
+      <c r="EJ5" s="0"/>
+      <c r="EK5" s="0"/>
+      <c r="EL5" s="0"/>
+      <c r="EM5" s="0"/>
+      <c r="EN5" s="0"/>
+      <c r="EO5" s="0"/>
+      <c r="EP5" s="0"/>
+      <c r="EQ5" s="0"/>
+      <c r="ER5" s="0"/>
+      <c r="ES5" s="0"/>
+      <c r="ET5" s="0"/>
+      <c r="EU5" s="0"/>
+      <c r="EV5" s="0"/>
+      <c r="EW5" s="0"/>
+      <c r="EX5" s="0"/>
+      <c r="EY5" s="0"/>
+      <c r="EZ5" s="0"/>
+      <c r="FA5" s="0"/>
+      <c r="FB5" s="0"/>
+      <c r="FC5" s="0"/>
+      <c r="FD5" s="0"/>
+      <c r="FE5" s="0"/>
+      <c r="FF5" s="0"/>
+      <c r="FG5" s="0"/>
+      <c r="FH5" s="0"/>
+      <c r="FI5" s="0"/>
+      <c r="FJ5" s="0"/>
+      <c r="FK5" s="0"/>
+      <c r="FL5" s="0"/>
+      <c r="FM5" s="0"/>
+      <c r="FN5" s="0"/>
+      <c r="FO5" s="0"/>
+      <c r="FP5" s="0"/>
+      <c r="FQ5" s="0"/>
+      <c r="FR5" s="0"/>
+      <c r="FS5" s="0"/>
+      <c r="FT5" s="0"/>
+      <c r="FU5" s="0"/>
+      <c r="FV5" s="0"/>
+      <c r="FW5" s="0"/>
+      <c r="FX5" s="0"/>
+      <c r="FY5" s="0"/>
+      <c r="FZ5" s="0"/>
+      <c r="GA5" s="0"/>
+      <c r="GB5" s="0"/>
+      <c r="GC5" s="0"/>
+      <c r="GD5" s="0"/>
+      <c r="GE5" s="0"/>
+      <c r="GF5" s="0"/>
+      <c r="GG5" s="0"/>
+      <c r="GH5" s="0"/>
+      <c r="GI5" s="0"/>
+      <c r="GJ5" s="0"/>
+      <c r="GK5" s="0"/>
+      <c r="GL5" s="0"/>
+      <c r="GM5" s="0"/>
+      <c r="GN5" s="0"/>
+      <c r="GO5" s="0"/>
+      <c r="GP5" s="0"/>
+      <c r="GQ5" s="0"/>
+      <c r="GR5" s="0"/>
+      <c r="GS5" s="0"/>
+      <c r="GT5" s="0"/>
+      <c r="GU5" s="0"/>
+      <c r="GV5" s="0"/>
+      <c r="GW5" s="0"/>
+      <c r="GX5" s="0"/>
+      <c r="GY5" s="0"/>
+      <c r="GZ5" s="0"/>
+      <c r="HA5" s="0"/>
+      <c r="HB5" s="0"/>
+      <c r="HC5" s="0"/>
+      <c r="HD5" s="0"/>
+      <c r="HE5" s="0"/>
+      <c r="HF5" s="0"/>
+      <c r="HG5" s="0"/>
+      <c r="HH5" s="0"/>
+      <c r="HI5" s="0"/>
+      <c r="HJ5" s="0"/>
+      <c r="HK5" s="0"/>
+      <c r="HL5" s="0"/>
+      <c r="HM5" s="0"/>
+      <c r="HN5" s="0"/>
+      <c r="HO5" s="0"/>
+      <c r="HP5" s="0"/>
+      <c r="HQ5" s="0"/>
+      <c r="HR5" s="0"/>
+      <c r="HS5" s="0"/>
+      <c r="HT5" s="0"/>
+      <c r="HU5" s="0"/>
+      <c r="HV5" s="0"/>
+      <c r="HW5" s="0"/>
+      <c r="HX5" s="0"/>
+      <c r="HY5" s="0"/>
+      <c r="HZ5" s="0"/>
+      <c r="IA5" s="0"/>
+      <c r="IB5" s="0"/>
+      <c r="IC5" s="0"/>
+      <c r="ID5" s="0"/>
+      <c r="IE5" s="0"/>
+      <c r="IF5" s="0"/>
+      <c r="IG5" s="0"/>
+      <c r="IH5" s="0"/>
+      <c r="II5" s="0"/>
+      <c r="IJ5" s="0"/>
+      <c r="IK5" s="0"/>
+      <c r="IL5" s="0"/>
+      <c r="IM5" s="0"/>
+      <c r="IN5" s="0"/>
+      <c r="IO5" s="0"/>
+      <c r="IP5" s="0"/>
+      <c r="IQ5" s="0"/>
+      <c r="IR5" s="0"/>
+      <c r="IS5" s="0"/>
+      <c r="IT5" s="0"/>
+      <c r="IU5" s="0"/>
+      <c r="IV5" s="0"/>
+      <c r="IW5" s="0"/>
+      <c r="IX5" s="0"/>
+      <c r="IY5" s="0"/>
+      <c r="IZ5" s="0"/>
+      <c r="JA5" s="0"/>
+      <c r="JB5" s="0"/>
+      <c r="JC5" s="0"/>
+      <c r="JD5" s="0"/>
+      <c r="JE5" s="0"/>
+      <c r="JF5" s="0"/>
+      <c r="JG5" s="0"/>
+      <c r="JH5" s="0"/>
+      <c r="JI5" s="0"/>
+      <c r="JJ5" s="0"/>
+      <c r="JK5" s="0"/>
+      <c r="JL5" s="0"/>
+      <c r="JM5" s="0"/>
+      <c r="JN5" s="0"/>
+      <c r="JO5" s="0"/>
+      <c r="JP5" s="0"/>
+      <c r="JQ5" s="0"/>
+      <c r="JR5" s="0"/>
+      <c r="JS5" s="0"/>
+      <c r="JT5" s="0"/>
+      <c r="JU5" s="0"/>
+      <c r="JV5" s="0"/>
+      <c r="JW5" s="0"/>
+      <c r="JX5" s="0"/>
+      <c r="JY5" s="0"/>
+      <c r="JZ5" s="0"/>
+      <c r="KA5" s="0"/>
+      <c r="KB5" s="0"/>
+      <c r="KC5" s="0"/>
+      <c r="KD5" s="0"/>
+      <c r="KE5" s="0"/>
+      <c r="KF5" s="0"/>
+      <c r="KG5" s="0"/>
+      <c r="KH5" s="0"/>
+      <c r="KI5" s="0"/>
+      <c r="KJ5" s="0"/>
+      <c r="KK5" s="0"/>
+      <c r="KL5" s="0"/>
+      <c r="KM5" s="0"/>
+      <c r="KN5" s="0"/>
+      <c r="KO5" s="0"/>
+      <c r="KP5" s="0"/>
+      <c r="KQ5" s="0"/>
+      <c r="KR5" s="0"/>
+      <c r="KS5" s="0"/>
+      <c r="KT5" s="0"/>
+      <c r="KU5" s="0"/>
+      <c r="KV5" s="0"/>
+      <c r="KW5" s="0"/>
+      <c r="KX5" s="0"/>
+      <c r="KY5" s="0"/>
+      <c r="KZ5" s="0"/>
+      <c r="LA5" s="0"/>
+      <c r="LB5" s="0"/>
+      <c r="LC5" s="0"/>
+      <c r="LD5" s="0"/>
+      <c r="LE5" s="0"/>
+      <c r="LF5" s="0"/>
+      <c r="LG5" s="0"/>
+      <c r="LH5" s="0"/>
+      <c r="LI5" s="0"/>
+      <c r="LJ5" s="0"/>
+      <c r="LK5" s="0"/>
+      <c r="LL5" s="0"/>
+      <c r="LM5" s="0"/>
+      <c r="LN5" s="0"/>
+      <c r="LO5" s="0"/>
+      <c r="LP5" s="0"/>
+      <c r="LQ5" s="0"/>
+      <c r="LR5" s="0"/>
+      <c r="LS5" s="0"/>
+      <c r="LT5" s="0"/>
+      <c r="LU5" s="0"/>
+      <c r="LV5" s="0"/>
+      <c r="LW5" s="0"/>
+      <c r="LX5" s="0"/>
+      <c r="LY5" s="0"/>
+      <c r="LZ5" s="0"/>
+      <c r="MA5" s="0"/>
+      <c r="MB5" s="0"/>
+      <c r="MC5" s="0"/>
+      <c r="MD5" s="0"/>
+      <c r="ME5" s="0"/>
+      <c r="MF5" s="0"/>
+      <c r="MG5" s="0"/>
+      <c r="MH5" s="0"/>
+      <c r="MI5" s="0"/>
+      <c r="MJ5" s="0"/>
+      <c r="MK5" s="0"/>
+      <c r="ML5" s="0"/>
+      <c r="MM5" s="0"/>
+      <c r="MN5" s="0"/>
+      <c r="MO5" s="0"/>
+      <c r="MP5" s="0"/>
+      <c r="MQ5" s="0"/>
+      <c r="MR5" s="0"/>
+      <c r="MS5" s="0"/>
+      <c r="MT5" s="0"/>
+      <c r="MU5" s="0"/>
+      <c r="MV5" s="0"/>
+      <c r="MW5" s="0"/>
+      <c r="MX5" s="0"/>
+      <c r="MY5" s="0"/>
+      <c r="MZ5" s="0"/>
+      <c r="NA5" s="0"/>
+      <c r="NB5" s="0"/>
+      <c r="NC5" s="0"/>
+      <c r="ND5" s="0"/>
+      <c r="NE5" s="0"/>
+      <c r="NF5" s="0"/>
+      <c r="NG5" s="0"/>
+      <c r="NH5" s="0"/>
+      <c r="NI5" s="0"/>
+      <c r="NJ5" s="0"/>
+      <c r="NK5" s="0"/>
+      <c r="NL5" s="0"/>
+      <c r="NM5" s="0"/>
+      <c r="NN5" s="0"/>
+      <c r="NO5" s="0"/>
+      <c r="NP5" s="0"/>
+      <c r="NQ5" s="0"/>
+      <c r="NR5" s="0"/>
+      <c r="NS5" s="0"/>
+      <c r="NT5" s="0"/>
+      <c r="NU5" s="0"/>
+      <c r="NV5" s="0"/>
+      <c r="NW5" s="0"/>
+      <c r="NX5" s="0"/>
+      <c r="NY5" s="0"/>
+      <c r="NZ5" s="0"/>
+      <c r="OA5" s="0"/>
+      <c r="OB5" s="0"/>
+      <c r="OC5" s="0"/>
+      <c r="OD5" s="0"/>
+      <c r="OE5" s="0"/>
+      <c r="OF5" s="0"/>
+      <c r="OG5" s="0"/>
+      <c r="OH5" s="0"/>
+      <c r="OI5" s="0"/>
+      <c r="OJ5" s="0"/>
+      <c r="OK5" s="0"/>
+      <c r="OL5" s="0"/>
+      <c r="OM5" s="0"/>
+      <c r="ON5" s="0"/>
+      <c r="OO5" s="0"/>
+      <c r="OP5" s="0"/>
+      <c r="OQ5" s="0"/>
+      <c r="OR5" s="0"/>
+      <c r="OS5" s="0"/>
+      <c r="OT5" s="0"/>
+      <c r="OU5" s="0"/>
+      <c r="OV5" s="0"/>
+      <c r="OW5" s="0"/>
+      <c r="OX5" s="0"/>
+      <c r="OY5" s="0"/>
+      <c r="OZ5" s="0"/>
+      <c r="PA5" s="0"/>
+      <c r="PB5" s="0"/>
+      <c r="PC5" s="0"/>
+      <c r="PD5" s="0"/>
+      <c r="PE5" s="0"/>
+      <c r="PF5" s="0"/>
+      <c r="PG5" s="0"/>
+      <c r="PH5" s="0"/>
+      <c r="PI5" s="0"/>
+      <c r="PJ5" s="0"/>
+      <c r="PK5" s="0"/>
+      <c r="PL5" s="0"/>
+      <c r="PM5" s="0"/>
+      <c r="PN5" s="0"/>
+      <c r="PO5" s="0"/>
+      <c r="PP5" s="0"/>
+      <c r="PQ5" s="0"/>
+      <c r="PR5" s="0"/>
+      <c r="PS5" s="0"/>
+      <c r="PT5" s="0"/>
+      <c r="PU5" s="0"/>
+      <c r="PV5" s="0"/>
+      <c r="PW5" s="0"/>
+      <c r="PX5" s="0"/>
+      <c r="PY5" s="0"/>
+      <c r="PZ5" s="0"/>
+      <c r="QA5" s="0"/>
+      <c r="QB5" s="0"/>
+      <c r="QC5" s="0"/>
+      <c r="QD5" s="0"/>
+      <c r="QE5" s="0"/>
+      <c r="QF5" s="0"/>
+      <c r="QG5" s="0"/>
+      <c r="QH5" s="0"/>
+      <c r="QI5" s="0"/>
+      <c r="QJ5" s="0"/>
+      <c r="QK5" s="0"/>
+      <c r="QL5" s="0"/>
+      <c r="QM5" s="0"/>
+      <c r="QN5" s="0"/>
+      <c r="QO5" s="0"/>
+      <c r="QP5" s="0"/>
+      <c r="QQ5" s="0"/>
+      <c r="QR5" s="0"/>
+      <c r="QS5" s="0"/>
+      <c r="QT5" s="0"/>
+      <c r="QU5" s="0"/>
+      <c r="QV5" s="0"/>
+      <c r="QW5" s="0"/>
+      <c r="QX5" s="0"/>
+      <c r="QY5" s="0"/>
+      <c r="QZ5" s="0"/>
+      <c r="RA5" s="0"/>
+      <c r="RB5" s="0"/>
+      <c r="RC5" s="0"/>
+      <c r="RD5" s="0"/>
+      <c r="RE5" s="0"/>
+      <c r="RF5" s="0"/>
+      <c r="RG5" s="0"/>
+      <c r="RH5" s="0"/>
+      <c r="RI5" s="0"/>
+      <c r="RJ5" s="0"/>
+      <c r="RK5" s="0"/>
+      <c r="RL5" s="0"/>
+      <c r="RM5" s="0"/>
+      <c r="RN5" s="0"/>
+      <c r="RO5" s="0"/>
+      <c r="RP5" s="0"/>
+      <c r="RQ5" s="0"/>
+      <c r="RR5" s="0"/>
+      <c r="RS5" s="0"/>
+      <c r="RT5" s="0"/>
+      <c r="RU5" s="0"/>
+      <c r="RV5" s="0"/>
+      <c r="RW5" s="0"/>
+      <c r="RX5" s="0"/>
+      <c r="RY5" s="0"/>
+      <c r="RZ5" s="0"/>
+      <c r="SA5" s="0"/>
+      <c r="SB5" s="0"/>
+      <c r="SC5" s="0"/>
+      <c r="SD5" s="0"/>
+      <c r="SE5" s="0"/>
+      <c r="SF5" s="0"/>
+      <c r="SG5" s="0"/>
+      <c r="SH5" s="0"/>
+      <c r="SI5" s="0"/>
+      <c r="SJ5" s="0"/>
+      <c r="SK5" s="0"/>
+      <c r="SL5" s="0"/>
+      <c r="SM5" s="0"/>
+      <c r="SN5" s="0"/>
+      <c r="SO5" s="0"/>
+      <c r="SP5" s="0"/>
+      <c r="SQ5" s="0"/>
+      <c r="SR5" s="0"/>
+      <c r="SS5" s="0"/>
+      <c r="ST5" s="0"/>
+      <c r="SU5" s="0"/>
+      <c r="SV5" s="0"/>
+      <c r="SW5" s="0"/>
+      <c r="SX5" s="0"/>
+      <c r="SY5" s="0"/>
+      <c r="SZ5" s="0"/>
+      <c r="TA5" s="0"/>
+      <c r="TB5" s="0"/>
+      <c r="TC5" s="0"/>
+      <c r="TD5" s="0"/>
+      <c r="TE5" s="0"/>
+      <c r="TF5" s="0"/>
+      <c r="TG5" s="0"/>
+      <c r="TH5" s="0"/>
+      <c r="TI5" s="0"/>
+      <c r="TJ5" s="0"/>
+      <c r="TK5" s="0"/>
+      <c r="TL5" s="0"/>
+      <c r="TM5" s="0"/>
+      <c r="TN5" s="0"/>
+      <c r="TO5" s="0"/>
+      <c r="TP5" s="0"/>
+      <c r="TQ5" s="0"/>
+      <c r="TR5" s="0"/>
+      <c r="TS5" s="0"/>
+      <c r="TT5" s="0"/>
+      <c r="TU5" s="0"/>
+      <c r="TV5" s="0"/>
+      <c r="TW5" s="0"/>
+      <c r="TX5" s="0"/>
+      <c r="TY5" s="0"/>
+      <c r="TZ5" s="0"/>
+      <c r="UA5" s="0"/>
+      <c r="UB5" s="0"/>
+      <c r="UC5" s="0"/>
+      <c r="UD5" s="0"/>
+      <c r="UE5" s="0"/>
+      <c r="UF5" s="0"/>
+      <c r="UG5" s="0"/>
+      <c r="UH5" s="0"/>
+      <c r="UI5" s="0"/>
+      <c r="UJ5" s="0"/>
+      <c r="UK5" s="0"/>
+      <c r="UL5" s="0"/>
+      <c r="UM5" s="0"/>
+      <c r="UN5" s="0"/>
+      <c r="UO5" s="0"/>
+      <c r="UP5" s="0"/>
+      <c r="UQ5" s="0"/>
+      <c r="UR5" s="0"/>
+      <c r="US5" s="0"/>
+      <c r="UT5" s="0"/>
+      <c r="UU5" s="0"/>
+      <c r="UV5" s="0"/>
+      <c r="UW5" s="0"/>
+      <c r="UX5" s="0"/>
+      <c r="UY5" s="0"/>
+      <c r="UZ5" s="0"/>
+      <c r="VA5" s="0"/>
+      <c r="VB5" s="0"/>
+      <c r="VC5" s="0"/>
+      <c r="VD5" s="0"/>
+      <c r="VE5" s="0"/>
+      <c r="VF5" s="0"/>
+      <c r="VG5" s="0"/>
+      <c r="VH5" s="0"/>
+      <c r="VI5" s="0"/>
+      <c r="VJ5" s="0"/>
+      <c r="VK5" s="0"/>
+      <c r="VL5" s="0"/>
+      <c r="VM5" s="0"/>
+      <c r="VN5" s="0"/>
+      <c r="VO5" s="0"/>
+      <c r="VP5" s="0"/>
+      <c r="VQ5" s="0"/>
+      <c r="VR5" s="0"/>
+      <c r="VS5" s="0"/>
+      <c r="VT5" s="0"/>
+      <c r="VU5" s="0"/>
+      <c r="VV5" s="0"/>
+      <c r="VW5" s="0"/>
+      <c r="VX5" s="0"/>
+      <c r="VY5" s="0"/>
+      <c r="VZ5" s="0"/>
+      <c r="WA5" s="0"/>
+      <c r="WB5" s="0"/>
+      <c r="WC5" s="0"/>
+      <c r="WD5" s="0"/>
+      <c r="WE5" s="0"/>
+      <c r="WF5" s="0"/>
+      <c r="WG5" s="0"/>
+      <c r="WH5" s="0"/>
+      <c r="WI5" s="0"/>
+      <c r="WJ5" s="0"/>
+      <c r="WK5" s="0"/>
+      <c r="WL5" s="0"/>
+      <c r="WM5" s="0"/>
+      <c r="WN5" s="0"/>
+      <c r="WO5" s="0"/>
+      <c r="WP5" s="0"/>
+      <c r="WQ5" s="0"/>
+      <c r="WR5" s="0"/>
+      <c r="WS5" s="0"/>
+      <c r="WT5" s="0"/>
+      <c r="WU5" s="0"/>
+      <c r="WV5" s="0"/>
+      <c r="WW5" s="0"/>
+      <c r="WX5" s="0"/>
+      <c r="WY5" s="0"/>
+      <c r="WZ5" s="0"/>
+      <c r="XA5" s="0"/>
+      <c r="XB5" s="0"/>
+      <c r="XC5" s="0"/>
+      <c r="XD5" s="0"/>
+      <c r="XE5" s="0"/>
+      <c r="XF5" s="0"/>
+      <c r="XG5" s="0"/>
+      <c r="XH5" s="0"/>
+      <c r="XI5" s="0"/>
+      <c r="XJ5" s="0"/>
+      <c r="XK5" s="0"/>
+      <c r="XL5" s="0"/>
+      <c r="XM5" s="0"/>
+      <c r="XN5" s="0"/>
+      <c r="XO5" s="0"/>
+      <c r="XP5" s="0"/>
+      <c r="XQ5" s="0"/>
+      <c r="XR5" s="0"/>
+      <c r="XS5" s="0"/>
+      <c r="XT5" s="0"/>
+      <c r="XU5" s="0"/>
+      <c r="XV5" s="0"/>
+      <c r="XW5" s="0"/>
+      <c r="XX5" s="0"/>
+      <c r="XY5" s="0"/>
+      <c r="XZ5" s="0"/>
+      <c r="YA5" s="0"/>
+      <c r="YB5" s="0"/>
+      <c r="YC5" s="0"/>
+      <c r="YD5" s="0"/>
+      <c r="YE5" s="0"/>
+      <c r="YF5" s="0"/>
+      <c r="YG5" s="0"/>
+      <c r="YH5" s="0"/>
+      <c r="YI5" s="0"/>
+      <c r="YJ5" s="0"/>
+      <c r="YK5" s="0"/>
+      <c r="YL5" s="0"/>
+      <c r="YM5" s="0"/>
+      <c r="YN5" s="0"/>
+      <c r="YO5" s="0"/>
+      <c r="YP5" s="0"/>
+      <c r="YQ5" s="0"/>
+      <c r="YR5" s="0"/>
+      <c r="YS5" s="0"/>
+      <c r="YT5" s="0"/>
+      <c r="YU5" s="0"/>
+      <c r="YV5" s="0"/>
+      <c r="YW5" s="0"/>
+      <c r="YX5" s="0"/>
+      <c r="YY5" s="0"/>
+      <c r="YZ5" s="0"/>
+      <c r="ZA5" s="0"/>
+      <c r="ZB5" s="0"/>
+      <c r="ZC5" s="0"/>
+      <c r="ZD5" s="0"/>
+      <c r="ZE5" s="0"/>
+      <c r="ZF5" s="0"/>
+      <c r="ZG5" s="0"/>
+      <c r="ZH5" s="0"/>
+      <c r="ZI5" s="0"/>
+      <c r="ZJ5" s="0"/>
+      <c r="ZK5" s="0"/>
+      <c r="ZL5" s="0"/>
+      <c r="ZM5" s="0"/>
+      <c r="ZN5" s="0"/>
+      <c r="ZO5" s="0"/>
+      <c r="ZP5" s="0"/>
+      <c r="ZQ5" s="0"/>
+      <c r="ZR5" s="0"/>
+      <c r="ZS5" s="0"/>
+      <c r="ZT5" s="0"/>
+      <c r="ZU5" s="0"/>
+      <c r="ZV5" s="0"/>
+      <c r="ZW5" s="0"/>
+      <c r="ZX5" s="0"/>
+      <c r="ZY5" s="0"/>
+      <c r="ZZ5" s="0"/>
+      <c r="AAA5" s="0"/>
+      <c r="AAB5" s="0"/>
+      <c r="AAC5" s="0"/>
+      <c r="AAD5" s="0"/>
+      <c r="AAE5" s="0"/>
+      <c r="AAF5" s="0"/>
+      <c r="AAG5" s="0"/>
+      <c r="AAH5" s="0"/>
+      <c r="AAI5" s="0"/>
+      <c r="AAJ5" s="0"/>
+      <c r="AAK5" s="0"/>
+      <c r="AAL5" s="0"/>
+      <c r="AAM5" s="0"/>
+      <c r="AAN5" s="0"/>
+      <c r="AAO5" s="0"/>
+      <c r="AAP5" s="0"/>
+      <c r="AAQ5" s="0"/>
+      <c r="AAR5" s="0"/>
+      <c r="AAS5" s="0"/>
+      <c r="AAT5" s="0"/>
+      <c r="AAU5" s="0"/>
+      <c r="AAV5" s="0"/>
+      <c r="AAW5" s="0"/>
+      <c r="AAX5" s="0"/>
+      <c r="AAY5" s="0"/>
+      <c r="AAZ5" s="0"/>
+      <c r="ABA5" s="0"/>
+      <c r="ABB5" s="0"/>
+      <c r="ABC5" s="0"/>
+      <c r="ABD5" s="0"/>
+      <c r="ABE5" s="0"/>
+      <c r="ABF5" s="0"/>
+      <c r="ABG5" s="0"/>
+      <c r="ABH5" s="0"/>
+      <c r="ABI5" s="0"/>
+      <c r="ABJ5" s="0"/>
+      <c r="ABK5" s="0"/>
+      <c r="ABL5" s="0"/>
+      <c r="ABM5" s="0"/>
+      <c r="ABN5" s="0"/>
+      <c r="ABO5" s="0"/>
+      <c r="ABP5" s="0"/>
+      <c r="ABQ5" s="0"/>
+      <c r="ABR5" s="0"/>
+      <c r="ABS5" s="0"/>
+      <c r="ABT5" s="0"/>
+      <c r="ABU5" s="0"/>
+      <c r="ABV5" s="0"/>
+      <c r="ABW5" s="0"/>
+      <c r="ABX5" s="0"/>
+      <c r="ABY5" s="0"/>
+      <c r="ABZ5" s="0"/>
+      <c r="ACA5" s="0"/>
+      <c r="ACB5" s="0"/>
+      <c r="ACC5" s="0"/>
+      <c r="ACD5" s="0"/>
+      <c r="ACE5" s="0"/>
+      <c r="ACF5" s="0"/>
+      <c r="ACG5" s="0"/>
+      <c r="ACH5" s="0"/>
+      <c r="ACI5" s="0"/>
+      <c r="ACJ5" s="0"/>
+      <c r="ACK5" s="0"/>
+      <c r="ACL5" s="0"/>
+      <c r="ACM5" s="0"/>
+      <c r="ACN5" s="0"/>
+      <c r="ACO5" s="0"/>
+      <c r="ACP5" s="0"/>
+      <c r="ACQ5" s="0"/>
+      <c r="ACR5" s="0"/>
+      <c r="ACS5" s="0"/>
+      <c r="ACT5" s="0"/>
+      <c r="ACU5" s="0"/>
+      <c r="ACV5" s="0"/>
+      <c r="ACW5" s="0"/>
+      <c r="ACX5" s="0"/>
+      <c r="ACY5" s="0"/>
+      <c r="ACZ5" s="0"/>
+      <c r="ADA5" s="0"/>
+      <c r="ADB5" s="0"/>
+      <c r="ADC5" s="0"/>
+      <c r="ADD5" s="0"/>
+      <c r="ADE5" s="0"/>
+      <c r="ADF5" s="0"/>
+      <c r="ADG5" s="0"/>
+      <c r="ADH5" s="0"/>
+      <c r="ADI5" s="0"/>
+      <c r="ADJ5" s="0"/>
+      <c r="ADK5" s="0"/>
+      <c r="ADL5" s="0"/>
+      <c r="ADM5" s="0"/>
+      <c r="ADN5" s="0"/>
+      <c r="ADO5" s="0"/>
+      <c r="ADP5" s="0"/>
+      <c r="ADQ5" s="0"/>
+      <c r="ADR5" s="0"/>
+      <c r="ADS5" s="0"/>
+      <c r="ADT5" s="0"/>
+      <c r="ADU5" s="0"/>
+      <c r="ADV5" s="0"/>
+      <c r="ADW5" s="0"/>
+      <c r="ADX5" s="0"/>
+      <c r="ADY5" s="0"/>
+      <c r="ADZ5" s="0"/>
+      <c r="AEA5" s="0"/>
+      <c r="AEB5" s="0"/>
+      <c r="AEC5" s="0"/>
+      <c r="AED5" s="0"/>
+      <c r="AEE5" s="0"/>
+      <c r="AEF5" s="0"/>
+      <c r="AEG5" s="0"/>
+      <c r="AEH5" s="0"/>
+      <c r="AEI5" s="0"/>
+      <c r="AEJ5" s="0"/>
+      <c r="AEK5" s="0"/>
+      <c r="AEL5" s="0"/>
+      <c r="AEM5" s="0"/>
+      <c r="AEN5" s="0"/>
+      <c r="AEO5" s="0"/>
+      <c r="AEP5" s="0"/>
+      <c r="AEQ5" s="0"/>
+      <c r="AER5" s="0"/>
+      <c r="AES5" s="0"/>
+      <c r="AET5" s="0"/>
+      <c r="AEU5" s="0"/>
+      <c r="AEV5" s="0"/>
+      <c r="AEW5" s="0"/>
+      <c r="AEX5" s="0"/>
+      <c r="AEY5" s="0"/>
+      <c r="AEZ5" s="0"/>
+      <c r="AFA5" s="0"/>
+      <c r="AFB5" s="0"/>
+      <c r="AFC5" s="0"/>
+      <c r="AFD5" s="0"/>
+      <c r="AFE5" s="0"/>
+      <c r="AFF5" s="0"/>
+      <c r="AFG5" s="0"/>
+      <c r="AFH5" s="0"/>
+      <c r="AFI5" s="0"/>
+      <c r="AFJ5" s="0"/>
+      <c r="AFK5" s="0"/>
+      <c r="AFL5" s="0"/>
+      <c r="AFM5" s="0"/>
+      <c r="AFN5" s="0"/>
+      <c r="AFO5" s="0"/>
+      <c r="AFP5" s="0"/>
+      <c r="AFQ5" s="0"/>
+      <c r="AFR5" s="0"/>
+      <c r="AFS5" s="0"/>
+      <c r="AFT5" s="0"/>
+      <c r="AFU5" s="0"/>
+      <c r="AFV5" s="0"/>
+      <c r="AFW5" s="0"/>
+      <c r="AFX5" s="0"/>
+      <c r="AFY5" s="0"/>
+      <c r="AFZ5" s="0"/>
+      <c r="AGA5" s="0"/>
+      <c r="AGB5" s="0"/>
+      <c r="AGC5" s="0"/>
+      <c r="AGD5" s="0"/>
+      <c r="AGE5" s="0"/>
+      <c r="AGF5" s="0"/>
+      <c r="AGG5" s="0"/>
+      <c r="AGH5" s="0"/>
+      <c r="AGI5" s="0"/>
+      <c r="AGJ5" s="0"/>
+      <c r="AGK5" s="0"/>
+      <c r="AGL5" s="0"/>
+      <c r="AGM5" s="0"/>
+      <c r="AGN5" s="0"/>
+      <c r="AGO5" s="0"/>
+      <c r="AGP5" s="0"/>
+      <c r="AGQ5" s="0"/>
+      <c r="AGR5" s="0"/>
+      <c r="AGS5" s="0"/>
+      <c r="AGT5" s="0"/>
+      <c r="AGU5" s="0"/>
+      <c r="AGV5" s="0"/>
+      <c r="AGW5" s="0"/>
+      <c r="AGX5" s="0"/>
+      <c r="AGY5" s="0"/>
+      <c r="AGZ5" s="0"/>
+      <c r="AHA5" s="0"/>
+      <c r="AHB5" s="0"/>
+      <c r="AHC5" s="0"/>
+      <c r="AHD5" s="0"/>
+      <c r="AHE5" s="0"/>
+      <c r="AHF5" s="0"/>
+      <c r="AHG5" s="0"/>
+      <c r="AHH5" s="0"/>
+      <c r="AHI5" s="0"/>
+      <c r="AHJ5" s="0"/>
+      <c r="AHK5" s="0"/>
+      <c r="AHL5" s="0"/>
+      <c r="AHM5" s="0"/>
+      <c r="AHN5" s="0"/>
+      <c r="AHO5" s="0"/>
+      <c r="AHP5" s="0"/>
+      <c r="AHQ5" s="0"/>
+      <c r="AHR5" s="0"/>
+      <c r="AHS5" s="0"/>
+      <c r="AHT5" s="0"/>
+      <c r="AHU5" s="0"/>
+      <c r="AHV5" s="0"/>
+      <c r="AHW5" s="0"/>
+      <c r="AHX5" s="0"/>
+      <c r="AHY5" s="0"/>
+      <c r="AHZ5" s="0"/>
+      <c r="AIA5" s="0"/>
+      <c r="AIB5" s="0"/>
+      <c r="AIC5" s="0"/>
+      <c r="AID5" s="0"/>
+      <c r="AIE5" s="0"/>
+      <c r="AIF5" s="0"/>
+      <c r="AIG5" s="0"/>
+      <c r="AIH5" s="0"/>
+      <c r="AII5" s="0"/>
+      <c r="AIJ5" s="0"/>
+      <c r="AIK5" s="0"/>
+      <c r="AIL5" s="0"/>
+      <c r="AIM5" s="0"/>
+      <c r="AIN5" s="0"/>
+      <c r="AIO5" s="0"/>
+      <c r="AIP5" s="0"/>
+      <c r="AIQ5" s="0"/>
+      <c r="AIR5" s="0"/>
+      <c r="AIS5" s="0"/>
+      <c r="AIT5" s="0"/>
+      <c r="AIU5" s="0"/>
+      <c r="AIV5" s="0"/>
+      <c r="AIW5" s="0"/>
+      <c r="AIX5" s="0"/>
+      <c r="AIY5" s="0"/>
+      <c r="AIZ5" s="0"/>
+      <c r="AJA5" s="0"/>
+      <c r="AJB5" s="0"/>
+      <c r="AJC5" s="0"/>
+      <c r="AJD5" s="0"/>
+      <c r="AJE5" s="0"/>
+      <c r="AJF5" s="0"/>
+      <c r="AJG5" s="0"/>
+      <c r="AJH5" s="0"/>
+      <c r="AJI5" s="0"/>
+      <c r="AJJ5" s="0"/>
+      <c r="AJK5" s="0"/>
+      <c r="AJL5" s="0"/>
+      <c r="AJM5" s="0"/>
+      <c r="AJN5" s="0"/>
+      <c r="AJO5" s="0"/>
+      <c r="AJP5" s="0"/>
+      <c r="AJQ5" s="0"/>
+      <c r="AJR5" s="0"/>
+      <c r="AJS5" s="0"/>
+      <c r="AJT5" s="0"/>
+      <c r="AJU5" s="0"/>
+      <c r="AJV5" s="0"/>
+      <c r="AJW5" s="0"/>
+      <c r="AJX5" s="0"/>
+      <c r="AJY5" s="0"/>
+      <c r="AJZ5" s="0"/>
+      <c r="AKA5" s="0"/>
+      <c r="AKB5" s="0"/>
+      <c r="AKC5" s="0"/>
+      <c r="AKD5" s="0"/>
+      <c r="AKE5" s="0"/>
+      <c r="AKF5" s="0"/>
+      <c r="AKG5" s="0"/>
+      <c r="AKH5" s="0"/>
+      <c r="AKI5" s="0"/>
+      <c r="AKJ5" s="0"/>
+      <c r="AKK5" s="0"/>
+      <c r="AKL5" s="0"/>
+      <c r="AKM5" s="0"/>
+      <c r="AKN5" s="0"/>
+      <c r="AKO5" s="0"/>
+      <c r="AKP5" s="0"/>
+      <c r="AKQ5" s="0"/>
+      <c r="AKR5" s="0"/>
+      <c r="AKS5" s="0"/>
+      <c r="AKT5" s="0"/>
+      <c r="AKU5" s="0"/>
+      <c r="AKV5" s="0"/>
+      <c r="AKW5" s="0"/>
+      <c r="AKX5" s="0"/>
+      <c r="AKY5" s="0"/>
+      <c r="AKZ5" s="0"/>
+      <c r="ALA5" s="0"/>
+      <c r="ALB5" s="0"/>
+      <c r="ALC5" s="0"/>
+      <c r="ALD5" s="0"/>
+      <c r="ALE5" s="0"/>
+      <c r="ALF5" s="0"/>
+      <c r="ALG5" s="0"/>
+      <c r="ALH5" s="0"/>
+      <c r="ALI5" s="0"/>
+      <c r="ALJ5" s="0"/>
+      <c r="ALK5" s="0"/>
+      <c r="ALL5" s="0"/>
+      <c r="ALM5" s="0"/>
+      <c r="ALN5" s="0"/>
+      <c r="ALO5" s="0"/>
+      <c r="ALP5" s="0"/>
+      <c r="ALQ5" s="0"/>
+      <c r="ALR5" s="0"/>
+      <c r="ALS5" s="0"/>
+      <c r="ALT5" s="0"/>
+      <c r="ALU5" s="0"/>
+      <c r="ALV5" s="0"/>
+      <c r="ALW5" s="0"/>
+      <c r="ALX5" s="0"/>
+      <c r="ALY5" s="0"/>
+      <c r="ALZ5" s="0"/>
+      <c r="AMA5" s="0"/>
+      <c r="AMB5" s="0"/>
+      <c r="AMC5" s="0"/>
+      <c r="AMD5" s="0"/>
+      <c r="AME5" s="0"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="H6" s="0"/>
       <c r="I6" s="0"/>
       <c r="J6" s="0"/>
       <c r="K6" s="0"/>
@@ -5645,18 +6637,17 @@
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="0"/>
       <c r="I7" s="0"/>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
@@ -6672,30 +7663,27 @@
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="F8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="H8" s="0"/>
       <c r="I8" s="0"/>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
@@ -7711,30 +8699,27 @@
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>19</v>
+      <c r="E9" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="H9" s="0"/>
       <c r="I9" s="0"/>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
@@ -8750,30 +9735,27 @@
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>19</v>
+      <c r="E10" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="H10" s="0"/>
       <c r="I10" s="0"/>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
@@ -9789,16 +10771,1039 @@
       <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
+      <c r="Q11" s="0"/>
+      <c r="R11" s="0"/>
+      <c r="S11" s="0"/>
+      <c r="T11" s="0"/>
+      <c r="U11" s="0"/>
+      <c r="V11" s="0"/>
+      <c r="W11" s="0"/>
+      <c r="X11" s="0"/>
+      <c r="Y11" s="0"/>
+      <c r="Z11" s="0"/>
+      <c r="AA11" s="0"/>
+      <c r="AB11" s="0"/>
+      <c r="AC11" s="0"/>
+      <c r="AD11" s="0"/>
+      <c r="AE11" s="0"/>
+      <c r="AF11" s="0"/>
+      <c r="AG11" s="0"/>
+      <c r="AH11" s="0"/>
+      <c r="AI11" s="0"/>
+      <c r="AJ11" s="0"/>
+      <c r="AK11" s="0"/>
+      <c r="AL11" s="0"/>
+      <c r="AM11" s="0"/>
+      <c r="AN11" s="0"/>
+      <c r="AO11" s="0"/>
+      <c r="AP11" s="0"/>
+      <c r="AQ11" s="0"/>
+      <c r="AR11" s="0"/>
+      <c r="AS11" s="0"/>
+      <c r="AT11" s="0"/>
+      <c r="AU11" s="0"/>
+      <c r="AV11" s="0"/>
+      <c r="AW11" s="0"/>
+      <c r="AX11" s="0"/>
+      <c r="AY11" s="0"/>
+      <c r="AZ11" s="0"/>
+      <c r="BA11" s="0"/>
+      <c r="BB11" s="0"/>
+      <c r="BC11" s="0"/>
+      <c r="BD11" s="0"/>
+      <c r="BE11" s="0"/>
+      <c r="BF11" s="0"/>
+      <c r="BG11" s="0"/>
+      <c r="BH11" s="0"/>
+      <c r="BI11" s="0"/>
+      <c r="BJ11" s="0"/>
+      <c r="BK11" s="0"/>
+      <c r="BL11" s="0"/>
+      <c r="BM11" s="0"/>
+      <c r="BN11" s="0"/>
+      <c r="BO11" s="0"/>
+      <c r="BP11" s="0"/>
+      <c r="BQ11" s="0"/>
+      <c r="BR11" s="0"/>
+      <c r="BS11" s="0"/>
+      <c r="BT11" s="0"/>
+      <c r="BU11" s="0"/>
+      <c r="BV11" s="0"/>
+      <c r="BW11" s="0"/>
+      <c r="BX11" s="0"/>
+      <c r="BY11" s="0"/>
+      <c r="BZ11" s="0"/>
+      <c r="CA11" s="0"/>
+      <c r="CB11" s="0"/>
+      <c r="CC11" s="0"/>
+      <c r="CD11" s="0"/>
+      <c r="CE11" s="0"/>
+      <c r="CF11" s="0"/>
+      <c r="CG11" s="0"/>
+      <c r="CH11" s="0"/>
+      <c r="CI11" s="0"/>
+      <c r="CJ11" s="0"/>
+      <c r="CK11" s="0"/>
+      <c r="CL11" s="0"/>
+      <c r="CM11" s="0"/>
+      <c r="CN11" s="0"/>
+      <c r="CO11" s="0"/>
+      <c r="CP11" s="0"/>
+      <c r="CQ11" s="0"/>
+      <c r="CR11" s="0"/>
+      <c r="CS11" s="0"/>
+      <c r="CT11" s="0"/>
+      <c r="CU11" s="0"/>
+      <c r="CV11" s="0"/>
+      <c r="CW11" s="0"/>
+      <c r="CX11" s="0"/>
+      <c r="CY11" s="0"/>
+      <c r="CZ11" s="0"/>
+      <c r="DA11" s="0"/>
+      <c r="DB11" s="0"/>
+      <c r="DC11" s="0"/>
+      <c r="DD11" s="0"/>
+      <c r="DE11" s="0"/>
+      <c r="DF11" s="0"/>
+      <c r="DG11" s="0"/>
+      <c r="DH11" s="0"/>
+      <c r="DI11" s="0"/>
+      <c r="DJ11" s="0"/>
+      <c r="DK11" s="0"/>
+      <c r="DL11" s="0"/>
+      <c r="DM11" s="0"/>
+      <c r="DN11" s="0"/>
+      <c r="DO11" s="0"/>
+      <c r="DP11" s="0"/>
+      <c r="DQ11" s="0"/>
+      <c r="DR11" s="0"/>
+      <c r="DS11" s="0"/>
+      <c r="DT11" s="0"/>
+      <c r="DU11" s="0"/>
+      <c r="DV11" s="0"/>
+      <c r="DW11" s="0"/>
+      <c r="DX11" s="0"/>
+      <c r="DY11" s="0"/>
+      <c r="DZ11" s="0"/>
+      <c r="EA11" s="0"/>
+      <c r="EB11" s="0"/>
+      <c r="EC11" s="0"/>
+      <c r="ED11" s="0"/>
+      <c r="EE11" s="0"/>
+      <c r="EF11" s="0"/>
+      <c r="EG11" s="0"/>
+      <c r="EH11" s="0"/>
+      <c r="EI11" s="0"/>
+      <c r="EJ11" s="0"/>
+      <c r="EK11" s="0"/>
+      <c r="EL11" s="0"/>
+      <c r="EM11" s="0"/>
+      <c r="EN11" s="0"/>
+      <c r="EO11" s="0"/>
+      <c r="EP11" s="0"/>
+      <c r="EQ11" s="0"/>
+      <c r="ER11" s="0"/>
+      <c r="ES11" s="0"/>
+      <c r="ET11" s="0"/>
+      <c r="EU11" s="0"/>
+      <c r="EV11" s="0"/>
+      <c r="EW11" s="0"/>
+      <c r="EX11" s="0"/>
+      <c r="EY11" s="0"/>
+      <c r="EZ11" s="0"/>
+      <c r="FA11" s="0"/>
+      <c r="FB11" s="0"/>
+      <c r="FC11" s="0"/>
+      <c r="FD11" s="0"/>
+      <c r="FE11" s="0"/>
+      <c r="FF11" s="0"/>
+      <c r="FG11" s="0"/>
+      <c r="FH11" s="0"/>
+      <c r="FI11" s="0"/>
+      <c r="FJ11" s="0"/>
+      <c r="FK11" s="0"/>
+      <c r="FL11" s="0"/>
+      <c r="FM11" s="0"/>
+      <c r="FN11" s="0"/>
+      <c r="FO11" s="0"/>
+      <c r="FP11" s="0"/>
+      <c r="FQ11" s="0"/>
+      <c r="FR11" s="0"/>
+      <c r="FS11" s="0"/>
+      <c r="FT11" s="0"/>
+      <c r="FU11" s="0"/>
+      <c r="FV11" s="0"/>
+      <c r="FW11" s="0"/>
+      <c r="FX11" s="0"/>
+      <c r="FY11" s="0"/>
+      <c r="FZ11" s="0"/>
+      <c r="GA11" s="0"/>
+      <c r="GB11" s="0"/>
+      <c r="GC11" s="0"/>
+      <c r="GD11" s="0"/>
+      <c r="GE11" s="0"/>
+      <c r="GF11" s="0"/>
+      <c r="GG11" s="0"/>
+      <c r="GH11" s="0"/>
+      <c r="GI11" s="0"/>
+      <c r="GJ11" s="0"/>
+      <c r="GK11" s="0"/>
+      <c r="GL11" s="0"/>
+      <c r="GM11" s="0"/>
+      <c r="GN11" s="0"/>
+      <c r="GO11" s="0"/>
+      <c r="GP11" s="0"/>
+      <c r="GQ11" s="0"/>
+      <c r="GR11" s="0"/>
+      <c r="GS11" s="0"/>
+      <c r="GT11" s="0"/>
+      <c r="GU11" s="0"/>
+      <c r="GV11" s="0"/>
+      <c r="GW11" s="0"/>
+      <c r="GX11" s="0"/>
+      <c r="GY11" s="0"/>
+      <c r="GZ11" s="0"/>
+      <c r="HA11" s="0"/>
+      <c r="HB11" s="0"/>
+      <c r="HC11" s="0"/>
+      <c r="HD11" s="0"/>
+      <c r="HE11" s="0"/>
+      <c r="HF11" s="0"/>
+      <c r="HG11" s="0"/>
+      <c r="HH11" s="0"/>
+      <c r="HI11" s="0"/>
+      <c r="HJ11" s="0"/>
+      <c r="HK11" s="0"/>
+      <c r="HL11" s="0"/>
+      <c r="HM11" s="0"/>
+      <c r="HN11" s="0"/>
+      <c r="HO11" s="0"/>
+      <c r="HP11" s="0"/>
+      <c r="HQ11" s="0"/>
+      <c r="HR11" s="0"/>
+      <c r="HS11" s="0"/>
+      <c r="HT11" s="0"/>
+      <c r="HU11" s="0"/>
+      <c r="HV11" s="0"/>
+      <c r="HW11" s="0"/>
+      <c r="HX11" s="0"/>
+      <c r="HY11" s="0"/>
+      <c r="HZ11" s="0"/>
+      <c r="IA11" s="0"/>
+      <c r="IB11" s="0"/>
+      <c r="IC11" s="0"/>
+      <c r="ID11" s="0"/>
+      <c r="IE11" s="0"/>
+      <c r="IF11" s="0"/>
+      <c r="IG11" s="0"/>
+      <c r="IH11" s="0"/>
+      <c r="II11" s="0"/>
+      <c r="IJ11" s="0"/>
+      <c r="IK11" s="0"/>
+      <c r="IL11" s="0"/>
+      <c r="IM11" s="0"/>
+      <c r="IN11" s="0"/>
+      <c r="IO11" s="0"/>
+      <c r="IP11" s="0"/>
+      <c r="IQ11" s="0"/>
+      <c r="IR11" s="0"/>
+      <c r="IS11" s="0"/>
+      <c r="IT11" s="0"/>
+      <c r="IU11" s="0"/>
+      <c r="IV11" s="0"/>
+      <c r="IW11" s="0"/>
+      <c r="IX11" s="0"/>
+      <c r="IY11" s="0"/>
+      <c r="IZ11" s="0"/>
+      <c r="JA11" s="0"/>
+      <c r="JB11" s="0"/>
+      <c r="JC11" s="0"/>
+      <c r="JD11" s="0"/>
+      <c r="JE11" s="0"/>
+      <c r="JF11" s="0"/>
+      <c r="JG11" s="0"/>
+      <c r="JH11" s="0"/>
+      <c r="JI11" s="0"/>
+      <c r="JJ11" s="0"/>
+      <c r="JK11" s="0"/>
+      <c r="JL11" s="0"/>
+      <c r="JM11" s="0"/>
+      <c r="JN11" s="0"/>
+      <c r="JO11" s="0"/>
+      <c r="JP11" s="0"/>
+      <c r="JQ11" s="0"/>
+      <c r="JR11" s="0"/>
+      <c r="JS11" s="0"/>
+      <c r="JT11" s="0"/>
+      <c r="JU11" s="0"/>
+      <c r="JV11" s="0"/>
+      <c r="JW11" s="0"/>
+      <c r="JX11" s="0"/>
+      <c r="JY11" s="0"/>
+      <c r="JZ11" s="0"/>
+      <c r="KA11" s="0"/>
+      <c r="KB11" s="0"/>
+      <c r="KC11" s="0"/>
+      <c r="KD11" s="0"/>
+      <c r="KE11" s="0"/>
+      <c r="KF11" s="0"/>
+      <c r="KG11" s="0"/>
+      <c r="KH11" s="0"/>
+      <c r="KI11" s="0"/>
+      <c r="KJ11" s="0"/>
+      <c r="KK11" s="0"/>
+      <c r="KL11" s="0"/>
+      <c r="KM11" s="0"/>
+      <c r="KN11" s="0"/>
+      <c r="KO11" s="0"/>
+      <c r="KP11" s="0"/>
+      <c r="KQ11" s="0"/>
+      <c r="KR11" s="0"/>
+      <c r="KS11" s="0"/>
+      <c r="KT11" s="0"/>
+      <c r="KU11" s="0"/>
+      <c r="KV11" s="0"/>
+      <c r="KW11" s="0"/>
+      <c r="KX11" s="0"/>
+      <c r="KY11" s="0"/>
+      <c r="KZ11" s="0"/>
+      <c r="LA11" s="0"/>
+      <c r="LB11" s="0"/>
+      <c r="LC11" s="0"/>
+      <c r="LD11" s="0"/>
+      <c r="LE11" s="0"/>
+      <c r="LF11" s="0"/>
+      <c r="LG11" s="0"/>
+      <c r="LH11" s="0"/>
+      <c r="LI11" s="0"/>
+      <c r="LJ11" s="0"/>
+      <c r="LK11" s="0"/>
+      <c r="LL11" s="0"/>
+      <c r="LM11" s="0"/>
+      <c r="LN11" s="0"/>
+      <c r="LO11" s="0"/>
+      <c r="LP11" s="0"/>
+      <c r="LQ11" s="0"/>
+      <c r="LR11" s="0"/>
+      <c r="LS11" s="0"/>
+      <c r="LT11" s="0"/>
+      <c r="LU11" s="0"/>
+      <c r="LV11" s="0"/>
+      <c r="LW11" s="0"/>
+      <c r="LX11" s="0"/>
+      <c r="LY11" s="0"/>
+      <c r="LZ11" s="0"/>
+      <c r="MA11" s="0"/>
+      <c r="MB11" s="0"/>
+      <c r="MC11" s="0"/>
+      <c r="MD11" s="0"/>
+      <c r="ME11" s="0"/>
+      <c r="MF11" s="0"/>
+      <c r="MG11" s="0"/>
+      <c r="MH11" s="0"/>
+      <c r="MI11" s="0"/>
+      <c r="MJ11" s="0"/>
+      <c r="MK11" s="0"/>
+      <c r="ML11" s="0"/>
+      <c r="MM11" s="0"/>
+      <c r="MN11" s="0"/>
+      <c r="MO11" s="0"/>
+      <c r="MP11" s="0"/>
+      <c r="MQ11" s="0"/>
+      <c r="MR11" s="0"/>
+      <c r="MS11" s="0"/>
+      <c r="MT11" s="0"/>
+      <c r="MU11" s="0"/>
+      <c r="MV11" s="0"/>
+      <c r="MW11" s="0"/>
+      <c r="MX11" s="0"/>
+      <c r="MY11" s="0"/>
+      <c r="MZ11" s="0"/>
+      <c r="NA11" s="0"/>
+      <c r="NB11" s="0"/>
+      <c r="NC11" s="0"/>
+      <c r="ND11" s="0"/>
+      <c r="NE11" s="0"/>
+      <c r="NF11" s="0"/>
+      <c r="NG11" s="0"/>
+      <c r="NH11" s="0"/>
+      <c r="NI11" s="0"/>
+      <c r="NJ11" s="0"/>
+      <c r="NK11" s="0"/>
+      <c r="NL11" s="0"/>
+      <c r="NM11" s="0"/>
+      <c r="NN11" s="0"/>
+      <c r="NO11" s="0"/>
+      <c r="NP11" s="0"/>
+      <c r="NQ11" s="0"/>
+      <c r="NR11" s="0"/>
+      <c r="NS11" s="0"/>
+      <c r="NT11" s="0"/>
+      <c r="NU11" s="0"/>
+      <c r="NV11" s="0"/>
+      <c r="NW11" s="0"/>
+      <c r="NX11" s="0"/>
+      <c r="NY11" s="0"/>
+      <c r="NZ11" s="0"/>
+      <c r="OA11" s="0"/>
+      <c r="OB11" s="0"/>
+      <c r="OC11" s="0"/>
+      <c r="OD11" s="0"/>
+      <c r="OE11" s="0"/>
+      <c r="OF11" s="0"/>
+      <c r="OG11" s="0"/>
+      <c r="OH11" s="0"/>
+      <c r="OI11" s="0"/>
+      <c r="OJ11" s="0"/>
+      <c r="OK11" s="0"/>
+      <c r="OL11" s="0"/>
+      <c r="OM11" s="0"/>
+      <c r="ON11" s="0"/>
+      <c r="OO11" s="0"/>
+      <c r="OP11" s="0"/>
+      <c r="OQ11" s="0"/>
+      <c r="OR11" s="0"/>
+      <c r="OS11" s="0"/>
+      <c r="OT11" s="0"/>
+      <c r="OU11" s="0"/>
+      <c r="OV11" s="0"/>
+      <c r="OW11" s="0"/>
+      <c r="OX11" s="0"/>
+      <c r="OY11" s="0"/>
+      <c r="OZ11" s="0"/>
+      <c r="PA11" s="0"/>
+      <c r="PB11" s="0"/>
+      <c r="PC11" s="0"/>
+      <c r="PD11" s="0"/>
+      <c r="PE11" s="0"/>
+      <c r="PF11" s="0"/>
+      <c r="PG11" s="0"/>
+      <c r="PH11" s="0"/>
+      <c r="PI11" s="0"/>
+      <c r="PJ11" s="0"/>
+      <c r="PK11" s="0"/>
+      <c r="PL11" s="0"/>
+      <c r="PM11" s="0"/>
+      <c r="PN11" s="0"/>
+      <c r="PO11" s="0"/>
+      <c r="PP11" s="0"/>
+      <c r="PQ11" s="0"/>
+      <c r="PR11" s="0"/>
+      <c r="PS11" s="0"/>
+      <c r="PT11" s="0"/>
+      <c r="PU11" s="0"/>
+      <c r="PV11" s="0"/>
+      <c r="PW11" s="0"/>
+      <c r="PX11" s="0"/>
+      <c r="PY11" s="0"/>
+      <c r="PZ11" s="0"/>
+      <c r="QA11" s="0"/>
+      <c r="QB11" s="0"/>
+      <c r="QC11" s="0"/>
+      <c r="QD11" s="0"/>
+      <c r="QE11" s="0"/>
+      <c r="QF11" s="0"/>
+      <c r="QG11" s="0"/>
+      <c r="QH11" s="0"/>
+      <c r="QI11" s="0"/>
+      <c r="QJ11" s="0"/>
+      <c r="QK11" s="0"/>
+      <c r="QL11" s="0"/>
+      <c r="QM11" s="0"/>
+      <c r="QN11" s="0"/>
+      <c r="QO11" s="0"/>
+      <c r="QP11" s="0"/>
+      <c r="QQ11" s="0"/>
+      <c r="QR11" s="0"/>
+      <c r="QS11" s="0"/>
+      <c r="QT11" s="0"/>
+      <c r="QU11" s="0"/>
+      <c r="QV11" s="0"/>
+      <c r="QW11" s="0"/>
+      <c r="QX11" s="0"/>
+      <c r="QY11" s="0"/>
+      <c r="QZ11" s="0"/>
+      <c r="RA11" s="0"/>
+      <c r="RB11" s="0"/>
+      <c r="RC11" s="0"/>
+      <c r="RD11" s="0"/>
+      <c r="RE11" s="0"/>
+      <c r="RF11" s="0"/>
+      <c r="RG11" s="0"/>
+      <c r="RH11" s="0"/>
+      <c r="RI11" s="0"/>
+      <c r="RJ11" s="0"/>
+      <c r="RK11" s="0"/>
+      <c r="RL11" s="0"/>
+      <c r="RM11" s="0"/>
+      <c r="RN11" s="0"/>
+      <c r="RO11" s="0"/>
+      <c r="RP11" s="0"/>
+      <c r="RQ11" s="0"/>
+      <c r="RR11" s="0"/>
+      <c r="RS11" s="0"/>
+      <c r="RT11" s="0"/>
+      <c r="RU11" s="0"/>
+      <c r="RV11" s="0"/>
+      <c r="RW11" s="0"/>
+      <c r="RX11" s="0"/>
+      <c r="RY11" s="0"/>
+      <c r="RZ11" s="0"/>
+      <c r="SA11" s="0"/>
+      <c r="SB11" s="0"/>
+      <c r="SC11" s="0"/>
+      <c r="SD11" s="0"/>
+      <c r="SE11" s="0"/>
+      <c r="SF11" s="0"/>
+      <c r="SG11" s="0"/>
+      <c r="SH11" s="0"/>
+      <c r="SI11" s="0"/>
+      <c r="SJ11" s="0"/>
+      <c r="SK11" s="0"/>
+      <c r="SL11" s="0"/>
+      <c r="SM11" s="0"/>
+      <c r="SN11" s="0"/>
+      <c r="SO11" s="0"/>
+      <c r="SP11" s="0"/>
+      <c r="SQ11" s="0"/>
+      <c r="SR11" s="0"/>
+      <c r="SS11" s="0"/>
+      <c r="ST11" s="0"/>
+      <c r="SU11" s="0"/>
+      <c r="SV11" s="0"/>
+      <c r="SW11" s="0"/>
+      <c r="SX11" s="0"/>
+      <c r="SY11" s="0"/>
+      <c r="SZ11" s="0"/>
+      <c r="TA11" s="0"/>
+      <c r="TB11" s="0"/>
+      <c r="TC11" s="0"/>
+      <c r="TD11" s="0"/>
+      <c r="TE11" s="0"/>
+      <c r="TF11" s="0"/>
+      <c r="TG11" s="0"/>
+      <c r="TH11" s="0"/>
+      <c r="TI11" s="0"/>
+      <c r="TJ11" s="0"/>
+      <c r="TK11" s="0"/>
+      <c r="TL11" s="0"/>
+      <c r="TM11" s="0"/>
+      <c r="TN11" s="0"/>
+      <c r="TO11" s="0"/>
+      <c r="TP11" s="0"/>
+      <c r="TQ11" s="0"/>
+      <c r="TR11" s="0"/>
+      <c r="TS11" s="0"/>
+      <c r="TT11" s="0"/>
+      <c r="TU11" s="0"/>
+      <c r="TV11" s="0"/>
+      <c r="TW11" s="0"/>
+      <c r="TX11" s="0"/>
+      <c r="TY11" s="0"/>
+      <c r="TZ11" s="0"/>
+      <c r="UA11" s="0"/>
+      <c r="UB11" s="0"/>
+      <c r="UC11" s="0"/>
+      <c r="UD11" s="0"/>
+      <c r="UE11" s="0"/>
+      <c r="UF11" s="0"/>
+      <c r="UG11" s="0"/>
+      <c r="UH11" s="0"/>
+      <c r="UI11" s="0"/>
+      <c r="UJ11" s="0"/>
+      <c r="UK11" s="0"/>
+      <c r="UL11" s="0"/>
+      <c r="UM11" s="0"/>
+      <c r="UN11" s="0"/>
+      <c r="UO11" s="0"/>
+      <c r="UP11" s="0"/>
+      <c r="UQ11" s="0"/>
+      <c r="UR11" s="0"/>
+      <c r="US11" s="0"/>
+      <c r="UT11" s="0"/>
+      <c r="UU11" s="0"/>
+      <c r="UV11" s="0"/>
+      <c r="UW11" s="0"/>
+      <c r="UX11" s="0"/>
+      <c r="UY11" s="0"/>
+      <c r="UZ11" s="0"/>
+      <c r="VA11" s="0"/>
+      <c r="VB11" s="0"/>
+      <c r="VC11" s="0"/>
+      <c r="VD11" s="0"/>
+      <c r="VE11" s="0"/>
+      <c r="VF11" s="0"/>
+      <c r="VG11" s="0"/>
+      <c r="VH11" s="0"/>
+      <c r="VI11" s="0"/>
+      <c r="VJ11" s="0"/>
+      <c r="VK11" s="0"/>
+      <c r="VL11" s="0"/>
+      <c r="VM11" s="0"/>
+      <c r="VN11" s="0"/>
+      <c r="VO11" s="0"/>
+      <c r="VP11" s="0"/>
+      <c r="VQ11" s="0"/>
+      <c r="VR11" s="0"/>
+      <c r="VS11" s="0"/>
+      <c r="VT11" s="0"/>
+      <c r="VU11" s="0"/>
+      <c r="VV11" s="0"/>
+      <c r="VW11" s="0"/>
+      <c r="VX11" s="0"/>
+      <c r="VY11" s="0"/>
+      <c r="VZ11" s="0"/>
+      <c r="WA11" s="0"/>
+      <c r="WB11" s="0"/>
+      <c r="WC11" s="0"/>
+      <c r="WD11" s="0"/>
+      <c r="WE11" s="0"/>
+      <c r="WF11" s="0"/>
+      <c r="WG11" s="0"/>
+      <c r="WH11" s="0"/>
+      <c r="WI11" s="0"/>
+      <c r="WJ11" s="0"/>
+      <c r="WK11" s="0"/>
+      <c r="WL11" s="0"/>
+      <c r="WM11" s="0"/>
+      <c r="WN11" s="0"/>
+      <c r="WO11" s="0"/>
+      <c r="WP11" s="0"/>
+      <c r="WQ11" s="0"/>
+      <c r="WR11" s="0"/>
+      <c r="WS11" s="0"/>
+      <c r="WT11" s="0"/>
+      <c r="WU11" s="0"/>
+      <c r="WV11" s="0"/>
+      <c r="WW11" s="0"/>
+      <c r="WX11" s="0"/>
+      <c r="WY11" s="0"/>
+      <c r="WZ11" s="0"/>
+      <c r="XA11" s="0"/>
+      <c r="XB11" s="0"/>
+      <c r="XC11" s="0"/>
+      <c r="XD11" s="0"/>
+      <c r="XE11" s="0"/>
+      <c r="XF11" s="0"/>
+      <c r="XG11" s="0"/>
+      <c r="XH11" s="0"/>
+      <c r="XI11" s="0"/>
+      <c r="XJ11" s="0"/>
+      <c r="XK11" s="0"/>
+      <c r="XL11" s="0"/>
+      <c r="XM11" s="0"/>
+      <c r="XN11" s="0"/>
+      <c r="XO11" s="0"/>
+      <c r="XP11" s="0"/>
+      <c r="XQ11" s="0"/>
+      <c r="XR11" s="0"/>
+      <c r="XS11" s="0"/>
+      <c r="XT11" s="0"/>
+      <c r="XU11" s="0"/>
+      <c r="XV11" s="0"/>
+      <c r="XW11" s="0"/>
+      <c r="XX11" s="0"/>
+      <c r="XY11" s="0"/>
+      <c r="XZ11" s="0"/>
+      <c r="YA11" s="0"/>
+      <c r="YB11" s="0"/>
+      <c r="YC11" s="0"/>
+      <c r="YD11" s="0"/>
+      <c r="YE11" s="0"/>
+      <c r="YF11" s="0"/>
+      <c r="YG11" s="0"/>
+      <c r="YH11" s="0"/>
+      <c r="YI11" s="0"/>
+      <c r="YJ11" s="0"/>
+      <c r="YK11" s="0"/>
+      <c r="YL11" s="0"/>
+      <c r="YM11" s="0"/>
+      <c r="YN11" s="0"/>
+      <c r="YO11" s="0"/>
+      <c r="YP11" s="0"/>
+      <c r="YQ11" s="0"/>
+      <c r="YR11" s="0"/>
+      <c r="YS11" s="0"/>
+      <c r="YT11" s="0"/>
+      <c r="YU11" s="0"/>
+      <c r="YV11" s="0"/>
+      <c r="YW11" s="0"/>
+      <c r="YX11" s="0"/>
+      <c r="YY11" s="0"/>
+      <c r="YZ11" s="0"/>
+      <c r="ZA11" s="0"/>
+      <c r="ZB11" s="0"/>
+      <c r="ZC11" s="0"/>
+      <c r="ZD11" s="0"/>
+      <c r="ZE11" s="0"/>
+      <c r="ZF11" s="0"/>
+      <c r="ZG11" s="0"/>
+      <c r="ZH11" s="0"/>
+      <c r="ZI11" s="0"/>
+      <c r="ZJ11" s="0"/>
+      <c r="ZK11" s="0"/>
+      <c r="ZL11" s="0"/>
+      <c r="ZM11" s="0"/>
+      <c r="ZN11" s="0"/>
+      <c r="ZO11" s="0"/>
+      <c r="ZP11" s="0"/>
+      <c r="ZQ11" s="0"/>
+      <c r="ZR11" s="0"/>
+      <c r="ZS11" s="0"/>
+      <c r="ZT11" s="0"/>
+      <c r="ZU11" s="0"/>
+      <c r="ZV11" s="0"/>
+      <c r="ZW11" s="0"/>
+      <c r="ZX11" s="0"/>
+      <c r="ZY11" s="0"/>
+      <c r="ZZ11" s="0"/>
+      <c r="AAA11" s="0"/>
+      <c r="AAB11" s="0"/>
+      <c r="AAC11" s="0"/>
+      <c r="AAD11" s="0"/>
+      <c r="AAE11" s="0"/>
+      <c r="AAF11" s="0"/>
+      <c r="AAG11" s="0"/>
+      <c r="AAH11" s="0"/>
+      <c r="AAI11" s="0"/>
+      <c r="AAJ11" s="0"/>
+      <c r="AAK11" s="0"/>
+      <c r="AAL11" s="0"/>
+      <c r="AAM11" s="0"/>
+      <c r="AAN11" s="0"/>
+      <c r="AAO11" s="0"/>
+      <c r="AAP11" s="0"/>
+      <c r="AAQ11" s="0"/>
+      <c r="AAR11" s="0"/>
+      <c r="AAS11" s="0"/>
+      <c r="AAT11" s="0"/>
+      <c r="AAU11" s="0"/>
+      <c r="AAV11" s="0"/>
+      <c r="AAW11" s="0"/>
+      <c r="AAX11" s="0"/>
+      <c r="AAY11" s="0"/>
+      <c r="AAZ11" s="0"/>
+      <c r="ABA11" s="0"/>
+      <c r="ABB11" s="0"/>
+      <c r="ABC11" s="0"/>
+      <c r="ABD11" s="0"/>
+      <c r="ABE11" s="0"/>
+      <c r="ABF11" s="0"/>
+      <c r="ABG11" s="0"/>
+      <c r="ABH11" s="0"/>
+      <c r="ABI11" s="0"/>
+      <c r="ABJ11" s="0"/>
+      <c r="ABK11" s="0"/>
+      <c r="ABL11" s="0"/>
+      <c r="ABM11" s="0"/>
+      <c r="ABN11" s="0"/>
+      <c r="ABO11" s="0"/>
+      <c r="ABP11" s="0"/>
+      <c r="ABQ11" s="0"/>
+      <c r="ABR11" s="0"/>
+      <c r="ABS11" s="0"/>
+      <c r="ABT11" s="0"/>
+      <c r="ABU11" s="0"/>
+      <c r="ABV11" s="0"/>
+      <c r="ABW11" s="0"/>
+      <c r="ABX11" s="0"/>
+      <c r="ABY11" s="0"/>
+      <c r="ABZ11" s="0"/>
+      <c r="ACA11" s="0"/>
+      <c r="ACB11" s="0"/>
+      <c r="ACC11" s="0"/>
+      <c r="ACD11" s="0"/>
+      <c r="ACE11" s="0"/>
+      <c r="ACF11" s="0"/>
+      <c r="ACG11" s="0"/>
+      <c r="ACH11" s="0"/>
+      <c r="ACI11" s="0"/>
+      <c r="ACJ11" s="0"/>
+      <c r="ACK11" s="0"/>
+      <c r="ACL11" s="0"/>
+      <c r="ACM11" s="0"/>
+      <c r="ACN11" s="0"/>
+      <c r="ACO11" s="0"/>
+      <c r="ACP11" s="0"/>
+      <c r="ACQ11" s="0"/>
+      <c r="ACR11" s="0"/>
+      <c r="ACS11" s="0"/>
+      <c r="ACT11" s="0"/>
+      <c r="ACU11" s="0"/>
+      <c r="ACV11" s="0"/>
+      <c r="ACW11" s="0"/>
+      <c r="ACX11" s="0"/>
+      <c r="ACY11" s="0"/>
+      <c r="ACZ11" s="0"/>
+      <c r="ADA11" s="0"/>
+      <c r="ADB11" s="0"/>
+      <c r="ADC11" s="0"/>
+      <c r="ADD11" s="0"/>
+      <c r="ADE11" s="0"/>
+      <c r="ADF11" s="0"/>
+      <c r="ADG11" s="0"/>
+      <c r="ADH11" s="0"/>
+      <c r="ADI11" s="0"/>
+      <c r="ADJ11" s="0"/>
+      <c r="ADK11" s="0"/>
+      <c r="ADL11" s="0"/>
+      <c r="ADM11" s="0"/>
+      <c r="ADN11" s="0"/>
+      <c r="ADO11" s="0"/>
+      <c r="ADP11" s="0"/>
+      <c r="ADQ11" s="0"/>
+      <c r="ADR11" s="0"/>
+      <c r="ADS11" s="0"/>
+      <c r="ADT11" s="0"/>
+      <c r="ADU11" s="0"/>
+      <c r="ADV11" s="0"/>
+      <c r="ADW11" s="0"/>
+      <c r="ADX11" s="0"/>
+      <c r="ADY11" s="0"/>
+      <c r="ADZ11" s="0"/>
+      <c r="AEA11" s="0"/>
+      <c r="AEB11" s="0"/>
+      <c r="AEC11" s="0"/>
+      <c r="AED11" s="0"/>
+      <c r="AEE11" s="0"/>
+      <c r="AEF11" s="0"/>
+      <c r="AEG11" s="0"/>
+      <c r="AEH11" s="0"/>
+      <c r="AEI11" s="0"/>
+      <c r="AEJ11" s="0"/>
+      <c r="AEK11" s="0"/>
+      <c r="AEL11" s="0"/>
+      <c r="AEM11" s="0"/>
+      <c r="AEN11" s="0"/>
+      <c r="AEO11" s="0"/>
+      <c r="AEP11" s="0"/>
+      <c r="AEQ11" s="0"/>
+      <c r="AER11" s="0"/>
+      <c r="AES11" s="0"/>
+      <c r="AET11" s="0"/>
+      <c r="AEU11" s="0"/>
+      <c r="AEV11" s="0"/>
+      <c r="AEW11" s="0"/>
+      <c r="AEX11" s="0"/>
+      <c r="AEY11" s="0"/>
+      <c r="AEZ11" s="0"/>
+      <c r="AFA11" s="0"/>
+      <c r="AFB11" s="0"/>
+      <c r="AFC11" s="0"/>
+      <c r="AFD11" s="0"/>
+      <c r="AFE11" s="0"/>
+      <c r="AFF11" s="0"/>
+      <c r="AFG11" s="0"/>
+      <c r="AFH11" s="0"/>
+      <c r="AFI11" s="0"/>
+      <c r="AFJ11" s="0"/>
+      <c r="AFK11" s="0"/>
+      <c r="AFL11" s="0"/>
+      <c r="AFM11" s="0"/>
+      <c r="AFN11" s="0"/>
+      <c r="AFO11" s="0"/>
+      <c r="AFP11" s="0"/>
+      <c r="AFQ11" s="0"/>
+      <c r="AFR11" s="0"/>
+      <c r="AFS11" s="0"/>
+      <c r="AFT11" s="0"/>
+      <c r="AFU11" s="0"/>
+      <c r="AFV11" s="0"/>
+      <c r="AFW11" s="0"/>
+      <c r="AFX11" s="0"/>
+      <c r="AFY11" s="0"/>
+      <c r="AFZ11" s="0"/>
+      <c r="AGA11" s="0"/>
+      <c r="AGB11" s="0"/>
+      <c r="AGC11" s="0"/>
+      <c r="AGD11" s="0"/>
+      <c r="AGE11" s="0"/>
+      <c r="AGF11" s="0"/>
+      <c r="AGG11" s="0"/>
+      <c r="AGH11" s="0"/>
+      <c r="AGI11" s="0"/>
+      <c r="AGJ11" s="0"/>
+      <c r="AGK11" s="0"/>
+      <c r="AGL11" s="0"/>
+      <c r="AGM11" s="0"/>
+      <c r="AGN11" s="0"/>
+      <c r="AGO11" s="0"/>
+      <c r="AGP11" s="0"/>
+      <c r="AGQ11" s="0"/>
+      <c r="AGR11" s="0"/>
+      <c r="AGS11" s="0"/>
+      <c r="AGT11" s="0"/>
+      <c r="AGU11" s="0"/>
+      <c r="AGV11" s="0"/>
+      <c r="AGW11" s="0"/>
+      <c r="AGX11" s="0"/>
+      <c r="AGY11" s="0"/>
+      <c r="AGZ11" s="0"/>
+      <c r="AHA11" s="0"/>
+      <c r="AHB11" s="0"/>
+      <c r="AHC11" s="0"/>
+      <c r="AHD11" s="0"/>
+      <c r="AHE11" s="0"/>
+      <c r="AHF11" s="0"/>
+      <c r="AHG11" s="0"/>
+      <c r="AHH11" s="0"/>
+      <c r="AHI11" s="0"/>
+      <c r="AHJ11" s="0"/>
+      <c r="AHK11" s="0"/>
+      <c r="AHL11" s="0"/>
+      <c r="AHM11" s="0"/>
+      <c r="AHN11" s="0"/>
+      <c r="AHO11" s="0"/>
+      <c r="AHP11" s="0"/>
+      <c r="AHQ11" s="0"/>
+      <c r="AHR11" s="0"/>
+      <c r="AHS11" s="0"/>
+      <c r="AHT11" s="0"/>
+      <c r="AHU11" s="0"/>
+      <c r="AHV11" s="0"/>
+      <c r="AHW11" s="0"/>
+      <c r="AHX11" s="0"/>
+      <c r="AHY11" s="0"/>
+      <c r="AHZ11" s="0"/>
+      <c r="AIA11" s="0"/>
+      <c r="AIB11" s="0"/>
+      <c r="AIC11" s="0"/>
+      <c r="AID11" s="0"/>
+      <c r="AIE11" s="0"/>
+      <c r="AIF11" s="0"/>
+      <c r="AIG11" s="0"/>
+      <c r="AIH11" s="0"/>
+      <c r="AII11" s="0"/>
+      <c r="AIJ11" s="0"/>
+      <c r="AIK11" s="0"/>
+      <c r="AIL11" s="0"/>
+      <c r="AIM11" s="0"/>
+      <c r="AIN11" s="0"/>
+      <c r="AIO11" s="0"/>
+      <c r="AIP11" s="0"/>
+      <c r="AIQ11" s="0"/>
+      <c r="AIR11" s="0"/>
+      <c r="AIS11" s="0"/>
+      <c r="AIT11" s="0"/>
+      <c r="AIU11" s="0"/>
+      <c r="AIV11" s="0"/>
+      <c r="AIW11" s="0"/>
+      <c r="AIX11" s="0"/>
+      <c r="AIY11" s="0"/>
+      <c r="AIZ11" s="0"/>
+      <c r="AJA11" s="0"/>
+      <c r="AJB11" s="0"/>
+      <c r="AJC11" s="0"/>
+      <c r="AJD11" s="0"/>
+      <c r="AJE11" s="0"/>
+      <c r="AJF11" s="0"/>
+      <c r="AJG11" s="0"/>
+      <c r="AJH11" s="0"/>
+      <c r="AJI11" s="0"/>
+      <c r="AJJ11" s="0"/>
+      <c r="AJK11" s="0"/>
+      <c r="AJL11" s="0"/>
+      <c r="AJM11" s="0"/>
+      <c r="AJN11" s="0"/>
+      <c r="AJO11" s="0"/>
+      <c r="AJP11" s="0"/>
+      <c r="AJQ11" s="0"/>
+      <c r="AJR11" s="0"/>
+      <c r="AJS11" s="0"/>
+      <c r="AJT11" s="0"/>
+      <c r="AJU11" s="0"/>
+      <c r="AJV11" s="0"/>
+      <c r="AJW11" s="0"/>
+      <c r="AJX11" s="0"/>
+      <c r="AJY11" s="0"/>
+      <c r="AJZ11" s="0"/>
+      <c r="AKA11" s="0"/>
+      <c r="AKB11" s="0"/>
+      <c r="AKC11" s="0"/>
+      <c r="AKD11" s="0"/>
+      <c r="AKE11" s="0"/>
+      <c r="AKF11" s="0"/>
+      <c r="AKG11" s="0"/>
+      <c r="AKH11" s="0"/>
+      <c r="AKI11" s="0"/>
+      <c r="AKJ11" s="0"/>
+      <c r="AKK11" s="0"/>
+      <c r="AKL11" s="0"/>
+      <c r="AKM11" s="0"/>
+      <c r="AKN11" s="0"/>
+      <c r="AKO11" s="0"/>
+      <c r="AKP11" s="0"/>
+      <c r="AKQ11" s="0"/>
+      <c r="AKR11" s="0"/>
+      <c r="AKS11" s="0"/>
+      <c r="AKT11" s="0"/>
+      <c r="AKU11" s="0"/>
+      <c r="AKV11" s="0"/>
+      <c r="AKW11" s="0"/>
+      <c r="AKX11" s="0"/>
+      <c r="AKY11" s="0"/>
+      <c r="AKZ11" s="0"/>
+      <c r="ALA11" s="0"/>
+      <c r="ALB11" s="0"/>
+      <c r="ALC11" s="0"/>
+      <c r="ALD11" s="0"/>
+      <c r="ALE11" s="0"/>
+      <c r="ALF11" s="0"/>
+      <c r="ALG11" s="0"/>
+      <c r="ALH11" s="0"/>
+      <c r="ALI11" s="0"/>
+      <c r="ALJ11" s="0"/>
+      <c r="ALK11" s="0"/>
+      <c r="ALL11" s="0"/>
+      <c r="ALM11" s="0"/>
+      <c r="ALN11" s="0"/>
+      <c r="ALO11" s="0"/>
+      <c r="ALP11" s="0"/>
+      <c r="ALQ11" s="0"/>
+      <c r="ALR11" s="0"/>
+      <c r="ALS11" s="0"/>
+      <c r="ALT11" s="0"/>
+      <c r="ALU11" s="0"/>
+      <c r="ALV11" s="0"/>
+      <c r="ALW11" s="0"/>
+      <c r="ALX11" s="0"/>
+      <c r="ALY11" s="0"/>
+      <c r="ALZ11" s="0"/>
+      <c r="AMA11" s="0"/>
+      <c r="AMB11" s="0"/>
+      <c r="AMC11" s="0"/>
+      <c r="AMD11" s="0"/>
+      <c r="AME11" s="0"/>
+      <c r="AMF11" s="0"/>
+      <c r="AMG11" s="0"/>
+      <c r="AMH11" s="0"/>
+      <c r="AMI11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="H12" s="0"/>
       <c r="I12" s="0"/>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -10814,18 +12819,17 @@
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="H13" s="0"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
@@ -11841,30 +13845,27 @@
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
-      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="H14" s="0"/>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
@@ -12880,30 +14881,27 @@
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>10</v>
+      <c r="F15" s="9" t="s">
+        <v>26</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="H15" s="0"/>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
       <c r="K15" s="0"/>
@@ -13919,30 +15917,27 @@
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
-      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>35</v>
+      <c r="E16" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="H16" s="0"/>
       <c r="I16" s="0"/>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
@@ -14958,7 +16953,6 @@
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
-      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
@@ -14967,7 +16961,7 @@
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
-      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
@@ -15983,18 +17977,17 @@
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
-      <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="5"/>
+      <c r="H18" s="0"/>
       <c r="I18" s="0"/>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
@@ -17010,30 +19003,27 @@
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
-      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>31</v>
+      <c r="E19" s="9" t="s">
+        <v>35</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>40</v>
+      <c r="F19" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="H19" s="0"/>
       <c r="I19" s="0"/>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
@@ -18049,30 +20039,27 @@
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
-      <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="H20" s="0"/>
       <c r="I20" s="0"/>
       <c r="J20" s="0"/>
       <c r="K20" s="0"/>
@@ -19088,30 +21075,27 @@
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
-      <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>10</v>
+      <c r="F21" s="8" t="s">
+        <v>40</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
       <c r="K21" s="0"/>
@@ -20127,24 +22111,23 @@
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
       <c r="AMI21" s="0"/>
-      <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8" t="s">
-        <v>49</v>
+      <c r="E22" s="8" t="s">
+        <v>42</v>
       </c>
-      <c r="G22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
@@ -21160,24 +23143,23 @@
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
-      <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="10" t="s">
-        <v>51</v>
+      <c r="E23" s="10" t="s">
+        <v>44</v>
       </c>
-      <c r="G23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
@@ -22193,7 +24175,6 @@
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
-      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
@@ -22202,7 +24183,7 @@
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="H24" s="0"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
@@ -23218,30 +25199,27 @@
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
-      <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>31</v>
+      <c r="E25" s="9" t="s">
+        <v>35</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>40</v>
+      <c r="F25" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="H25" s="0"/>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
@@ -24257,30 +26235,27 @@
       <c r="AMG25" s="0"/>
       <c r="AMH25" s="0"/>
       <c r="AMI25" s="0"/>
-      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>42</v>
+      <c r="E26" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="H26" s="0"/>
       <c r="I26" s="0"/>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
@@ -25296,30 +27271,27 @@
       <c r="AMG26" s="0"/>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
-      <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>45</v>
+      <c r="E27" s="10" t="s">
+        <v>48</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>55</v>
+      <c r="F27" s="9" t="s">
+        <v>49</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="H27" s="0"/>
       <c r="I27" s="0"/>
       <c r="J27" s="0"/>
       <c r="K27" s="0"/>
@@ -26335,24 +28307,23 @@
       <c r="AMG27" s="0"/>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
-      <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="9" t="s">
-        <v>57</v>
+      <c r="E28" s="9" t="s">
+        <v>50</v>
       </c>
-      <c r="G28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="H28" s="0"/>
       <c r="I28" s="0"/>
       <c r="J28" s="0"/>
       <c r="K28" s="0"/>
@@ -27368,24 +29339,23 @@
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
-      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="10" t="s">
-        <v>51</v>
+      <c r="E29" s="10" t="s">
+        <v>44</v>
       </c>
-      <c r="G29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="H29" s="0"/>
       <c r="I29" s="0"/>
       <c r="J29" s="0"/>
       <c r="K29" s="0"/>
@@ -28401,7 +30371,6 @@
       <c r="AMG29" s="0"/>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
-      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
@@ -28410,7 +30379,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+      <c r="H30" s="0"/>
       <c r="I30" s="0"/>
       <c r="J30" s="0"/>
       <c r="K30" s="0"/>
@@ -29426,30 +31395,27 @@
       <c r="AMG30" s="0"/>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
-      <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>31</v>
+      <c r="E31" s="9" t="s">
+        <v>35</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>40</v>
+      <c r="F31" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="G31" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="H31" s="0"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
@@ -30465,30 +32431,27 @@
       <c r="AMG31" s="0"/>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
-      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>42</v>
+      <c r="E32" s="10" t="s">
+        <v>52</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>59</v>
+      <c r="F32" s="9" t="s">
+        <v>53</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="H32" s="0"/>
       <c r="I32" s="0"/>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
@@ -31504,30 +33467,27 @@
       <c r="AMG32" s="0"/>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
-      <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>45</v>
+      <c r="E33" s="10" t="s">
+        <v>54</v>
       </c>
-      <c r="F33" s="10" t="s">
-        <v>61</v>
+      <c r="F33" s="9" t="s">
+        <v>55</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="H33" s="0"/>
       <c r="I33" s="0"/>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
@@ -32543,24 +34503,23 @@
       <c r="AMG33" s="0"/>
       <c r="AMH33" s="0"/>
       <c r="AMI33" s="0"/>
-      <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D34" s="0"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="11" t="s">
-        <v>58</v>
+      <c r="E34" s="11" t="s">
+        <v>51</v>
       </c>
-      <c r="G34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="H34" s="0"/>
       <c r="I34" s="0"/>
       <c r="J34" s="0"/>
       <c r="K34" s="0"/>
@@ -33576,24 +35535,23 @@
       <c r="AMG34" s="0"/>
       <c r="AMH34" s="0"/>
       <c r="AMI34" s="0"/>
-      <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="10" t="s">
-        <v>51</v>
+      <c r="E35" s="10" t="s">
+        <v>44</v>
       </c>
-      <c r="G35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="H35" s="0"/>
       <c r="I35" s="0"/>
       <c r="J35" s="0"/>
       <c r="K35" s="0"/>
@@ -34609,7 +36567,6 @@
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
       <c r="AMI35" s="0"/>
-      <c r="AMJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
@@ -34618,7 +36575,7 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
+      <c r="H36" s="0"/>
       <c r="I36" s="0"/>
       <c r="J36" s="0"/>
       <c r="K36" s="0"/>
@@ -35634,30 +37591,27 @@
       <c r="AMG36" s="0"/>
       <c r="AMH36" s="0"/>
       <c r="AMI36" s="0"/>
-      <c r="AMJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>64</v>
+      <c r="E37" s="9" t="s">
+        <v>57</v>
       </c>
-      <c r="F37" s="9" t="s">
-        <v>65</v>
+      <c r="F37" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="G37" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="H37" s="0"/>
       <c r="I37" s="0"/>
       <c r="J37" s="0"/>
       <c r="K37" s="0"/>
@@ -36673,7 +38627,6 @@
       <c r="AMG37" s="0"/>
       <c r="AMH37" s="0"/>
       <c r="AMI37" s="0"/>
-      <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
@@ -36682,7 +38635,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
+      <c r="H38" s="0"/>
       <c r="I38" s="0"/>
       <c r="J38" s="0"/>
       <c r="K38" s="0"/>
@@ -37698,18 +39651,17 @@
       <c r="AMG38" s="0"/>
       <c r="AMH38" s="0"/>
       <c r="AMI38" s="0"/>
-      <c r="AMJ38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="5"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="5"/>
+      <c r="H39" s="0"/>
       <c r="I39" s="0"/>
       <c r="J39" s="0"/>
       <c r="K39" s="0"/>
@@ -38725,16 +40677,15 @@
       <c r="AMG39" s="0"/>
       <c r="AMH39" s="0"/>
       <c r="AMI39" s="0"/>
-      <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
+      <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
+      <c r="H40" s="0"/>
       <c r="I40" s="0"/>
       <c r="J40" s="0"/>
       <c r="K40" s="0"/>
@@ -39750,16 +41701,15 @@
       <c r="AMG40" s="0"/>
       <c r="AMH40" s="0"/>
       <c r="AMI40" s="0"/>
-      <c r="AMJ40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
+      <c r="E41" s="9"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
+      <c r="H41" s="0"/>
       <c r="I41" s="0"/>
       <c r="J41" s="0"/>
       <c r="K41" s="0"/>
@@ -40775,16 +42725,15 @@
       <c r="AMG41" s="0"/>
       <c r="AMH41" s="0"/>
       <c r="AMI41" s="0"/>
-      <c r="AMJ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
+      <c r="E42" s="9"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="H42" s="0"/>
       <c r="I42" s="0"/>
       <c r="J42" s="0"/>
       <c r="K42" s="0"/>
@@ -41800,18 +43749,17 @@
       <c r="AMG42" s="0"/>
       <c r="AMH42" s="0"/>
       <c r="AMI42" s="0"/>
-      <c r="AMJ42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="5"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="5"/>
+      <c r="H43" s="0"/>
       <c r="I43" s="0"/>
       <c r="J43" s="0"/>
       <c r="K43" s="0"/>
@@ -42827,30 +44775,27 @@
       <c r="AMG43" s="0"/>
       <c r="AMH43" s="0"/>
       <c r="AMI43" s="0"/>
-      <c r="AMJ43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>31</v>
+      <c r="E44" s="9" t="s">
+        <v>62</v>
       </c>
-      <c r="F44" s="9" t="s">
-        <v>70</v>
+      <c r="F44" s="8" t="s">
+        <v>63</v>
       </c>
-      <c r="G44" s="8" t="s">
-        <v>71</v>
-      </c>
+      <c r="H44" s="0"/>
       <c r="I44" s="0"/>
       <c r="J44" s="0"/>
       <c r="K44" s="0"/>
@@ -43866,30 +45811,27 @@
       <c r="AMG44" s="0"/>
       <c r="AMH44" s="0"/>
       <c r="AMI44" s="0"/>
-      <c r="AMJ44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>31</v>
+      <c r="E45" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
-      <c r="G45" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="H45" s="0"/>
       <c r="I45" s="0"/>
       <c r="J45" s="0"/>
       <c r="K45" s="0"/>
@@ -44905,7 +46847,6 @@
       <c r="AMG45" s="0"/>
       <c r="AMH45" s="0"/>
       <c r="AMI45" s="0"/>
-      <c r="AMJ45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7"/>
@@ -44914,7 +46855,7 @@
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
+      <c r="H46" s="0"/>
       <c r="I46" s="0"/>
       <c r="J46" s="0"/>
       <c r="K46" s="0"/>
@@ -45930,16 +47871,15 @@
       <c r="AMG46" s="0"/>
       <c r="AMH46" s="0"/>
       <c r="AMI46" s="0"/>
-      <c r="AMJ46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="8"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="8"/>
+      <c r="H47" s="0"/>
       <c r="I47" s="0"/>
       <c r="J47" s="0"/>
       <c r="K47" s="0"/>
@@ -46955,15 +48895,15 @@
       <c r="AMG47" s="0"/>
       <c r="AMH47" s="0"/>
       <c r="AMI47" s="0"/>
-      <c r="AMJ47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
+      <c r="E48" s="11"/>
       <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
+      <c r="H48" s="0"/>
       <c r="I48" s="0"/>
       <c r="J48" s="0"/>
       <c r="K48" s="0"/>
@@ -47979,7 +49919,6 @@
       <c r="AMG48" s="0"/>
       <c r="AMH48" s="0"/>
       <c r="AMI48" s="0"/>
-      <c r="AMJ48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
@@ -47988,7 +49927,7 @@
       <c r="D49" s="0"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
-      <c r="G49" s="0"/>
+      <c r="H49" s="0"/>
       <c r="I49" s="0"/>
       <c r="J49" s="0"/>
       <c r="K49" s="0"/>
@@ -49004,18 +50943,17 @@
       <c r="AMG49" s="0"/>
       <c r="AMH49" s="0"/>
       <c r="AMI49" s="0"/>
-      <c r="AMJ49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="5"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="5"/>
+      <c r="H50" s="0"/>
       <c r="I50" s="0"/>
       <c r="J50" s="0"/>
       <c r="K50" s="0"/>
@@ -50031,7 +51969,6 @@
       <c r="AMG50" s="0"/>
       <c r="AMH50" s="0"/>
       <c r="AMI50" s="0"/>
-      <c r="AMJ50" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fixing annotations for tests
</commit_message>
<xml_diff>
--- a/sbmlutils/dfba/diauxic_growth/annotations.xlsx
+++ b/sbmlutils/dfba/diauxic_growth/annotations.xlsx
@@ -193,7 +193,7 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">omit/MI:0018723</t>
+    <t xml:space="preserve">omim/MI:0018723</t>
   </si>
   <si>
     <t xml:space="preserve"># parameters</t>
@@ -452,7 +452,7 @@
   <dimension ref="A1:AMI50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>